<commit_message>
Sending table_1_22.xlsx - try 1 ^_^
</commit_message>
<xml_diff>
--- a/LR3/table_1_22.xlsx
+++ b/LR3/table_1_22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FE52D45-EA38-43D6-B4D9-486965C132A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{625580C4-41BC-4D08-8EF2-8E79D7625A56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -174,16 +174,16 @@
     <t>Тариф, руб./кв.м.</t>
   </si>
   <si>
-    <t>Общая сумма графы "Итого", руб.</t>
+    <t>средняя площадь, кв.м.</t>
   </si>
   <si>
-    <t>Средняя площадь, кв.м</t>
+    <t>максимальный срок просрочки, дней</t>
   </si>
   <si>
-    <t>Максимальный срок просрочки, дней</t>
+    <t>максимальная сумма к оплате, руб.</t>
   </si>
   <si>
-    <t>Максимальная сумма к оплате, руб.</t>
+    <t>общая сумма графы “Итого”, руб.</t>
   </si>
 </sst>
 </file>
@@ -529,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD201"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V26" sqref="V26"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3806,7 +3806,7 @@
     <row r="40" spans="1:56" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C40" s="5">
         <f>SUM(K3:K38)</f>
@@ -3869,7 +3869,7 @@
     <row r="41" spans="1:56" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C41" s="2">
         <f>AVERAGE(C3:C38)</f>
@@ -3932,7 +3932,7 @@
     <row r="42" spans="1:56" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C42" s="2">
         <f>MAX(H3:H38)</f>
@@ -3995,7 +3995,7 @@
     <row r="43" spans="1:56" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C43" s="2">
         <f>MAX(K3:K38)</f>

</xml_diff>

<commit_message>
Sending table_1_22.xlsx - try 2 ^_^
</commit_message>
<xml_diff>
--- a/LR3/table_1_22.xlsx
+++ b/LR3/table_1_22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{625580C4-41BC-4D08-8EF2-8E79D7625A56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A46ADF-B6F1-48B7-859A-93E321CCB720}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -183,7 +183,7 @@
     <t>максимальная сумма к оплате, руб.</t>
   </si>
   <si>
-    <t>общая сумма графы “Итого”, руб.</t>
+    <t>общая сумма графы "Итого", руб.</t>
   </si>
 </sst>
 </file>
@@ -529,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Sending table_1_22.xlsxl - try 3 ._.
</commit_message>
<xml_diff>
--- a/LR3/table_1_22.xlsx
+++ b/LR3/table_1_22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A46ADF-B6F1-48B7-859A-93E321CCB720}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9ABF0B9E-E09E-42AD-92B1-7FAC87008ABE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -530,7 +530,7 @@
   <dimension ref="A1:BD201"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Sending 1_22_xlsx - try 4
</commit_message>
<xml_diff>
--- a/LR3/table_1_22.xlsx
+++ b/LR3/table_1_22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9ABF0B9E-E09E-42AD-92B1-7FAC87008ABE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7FF15F9-E46D-41BB-AF23-FFC8D794C820}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,7 +190,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,6 +210,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -232,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -247,6 +254,7 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -529,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD201"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -772,6 +780,7 @@
     </row>
     <row r="4" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
+        <f>A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -857,6 +866,7 @@
     </row>
     <row r="5" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
+        <f t="shared" ref="A5:A38" si="5">A4+1</f>
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -942,6 +952,7 @@
     </row>
     <row r="6" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1027,6 +1038,7 @@
     </row>
     <row r="7" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1112,6 +1124,7 @@
     </row>
     <row r="8" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1197,6 +1210,7 @@
     </row>
     <row r="9" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1282,6 +1296,7 @@
     </row>
     <row r="10" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1367,6 +1382,7 @@
     </row>
     <row r="11" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1452,6 +1468,7 @@
     </row>
     <row r="12" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1537,6 +1554,7 @@
     </row>
     <row r="13" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1622,6 +1640,7 @@
     </row>
     <row r="14" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1707,6 +1726,7 @@
     </row>
     <row r="15" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -1792,6 +1812,7 @@
     </row>
     <row r="16" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -1877,6 +1898,7 @@
     </row>
     <row r="17" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -1962,6 +1984,7 @@
     </row>
     <row r="18" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -2047,6 +2070,7 @@
     </row>
     <row r="19" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -2132,6 +2156,7 @@
     </row>
     <row r="20" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -2217,6 +2242,7 @@
     </row>
     <row r="21" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -2302,6 +2328,7 @@
     </row>
     <row r="22" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -2387,6 +2414,7 @@
     </row>
     <row r="23" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -2472,6 +2500,7 @@
     </row>
     <row r="24" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
+        <f t="shared" si="5"/>
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -2557,6 +2586,7 @@
     </row>
     <row r="25" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
+        <f t="shared" si="5"/>
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -2642,6 +2672,7 @@
     </row>
     <row r="26" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -2727,6 +2758,7 @@
     </row>
     <row r="27" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -2812,6 +2844,7 @@
     </row>
     <row r="28" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
+        <f t="shared" si="5"/>
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -2897,6 +2930,7 @@
     </row>
     <row r="29" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
+        <f t="shared" si="5"/>
         <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -2982,6 +3016,7 @@
     </row>
     <row r="30" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -3067,6 +3102,7 @@
     </row>
     <row r="31" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
+        <f t="shared" si="5"/>
         <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -3152,6 +3188,7 @@
     </row>
     <row r="32" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -3237,6 +3274,7 @@
     </row>
     <row r="33" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
+        <f t="shared" si="5"/>
         <v>31</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -3322,6 +3360,7 @@
     </row>
     <row r="34" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
+        <f t="shared" si="5"/>
         <v>32</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -3407,6 +3446,7 @@
     </row>
     <row r="35" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
+        <f t="shared" si="5"/>
         <v>33</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -3492,6 +3532,7 @@
     </row>
     <row r="36" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
+        <f t="shared" si="5"/>
         <v>34</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -3501,7 +3542,7 @@
         <v>53.5</v>
       </c>
       <c r="D36" s="2">
-        <f t="shared" ref="D36:D38" si="5">22*1.1/2</f>
+        <f t="shared" ref="D36:D38" si="6">22*1.1/2</f>
         <v>12.100000000000001</v>
       </c>
       <c r="E36" s="2">
@@ -3577,6 +3618,7 @@
     </row>
     <row r="37" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
+        <f t="shared" si="5"/>
         <v>35</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -3586,7 +3628,7 @@
         <v>53</v>
       </c>
       <c r="D37" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12.100000000000001</v>
       </c>
       <c r="E37" s="2">
@@ -3662,6 +3704,7 @@
     </row>
     <row r="38" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
+        <f t="shared" si="5"/>
         <v>36</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -3671,7 +3714,7 @@
         <v>52.5</v>
       </c>
       <c r="D38" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12.100000000000001</v>
       </c>
       <c r="E38" s="2">
@@ -4057,6 +4100,9 @@
     </row>
     <row r="44" spans="1:56" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
@@ -4112,6 +4158,9 @@
     </row>
     <row r="45" spans="1:56" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>

</xml_diff>

<commit_message>
Sending 1_22_xlsx - try 5
</commit_message>
<xml_diff>
--- a/LR3/table_1_22.xlsx
+++ b/LR3/table_1_22.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7FF15F9-E46D-41BB-AF23-FFC8D794C820}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{52F15052-81F0-405E-AF9F-C03F2F2F9F15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5484" yWindow="2172" windowWidth="18912" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,15 +34,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>№ квартиры</t>
-  </si>
-  <si>
-    <t>Фамилия квартиросъемщика</t>
-  </si>
-  <si>
-    <t>Срок оплаты</t>
-  </si>
-  <si>
-    <t>Дата оплаты</t>
   </si>
   <si>
     <t>Куропаткин 1</t>
@@ -185,6 +176,15 @@
   <si>
     <t>общая сумма графы "Итого", руб.</t>
   </si>
+  <si>
+    <t>Фамилия квартиросъёмщика</t>
+  </si>
+  <si>
+    <t>Срок оплаты, день</t>
+  </si>
+  <si>
+    <t>Дата оплаты, день</t>
+  </si>
 </sst>
 </file>
 
@@ -239,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -255,6 +255,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -537,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD201"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="57" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -618,34 +624,34 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -697,8 +703,8 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>21</v>
+      <c r="B3" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="C3" s="2">
         <v>70</v>
@@ -708,7 +714,7 @@
         <v>24.200000000000003</v>
       </c>
       <c r="E3" s="2">
-        <f>C3*D3</f>
+        <f>D3*C3</f>
         <v>1694.0000000000002</v>
       </c>
       <c r="F3" s="4">
@@ -718,18 +724,18 @@
         <v>44805</v>
       </c>
       <c r="H3" s="2">
-        <f>IF(G3&lt;=F3,0,A3-$A$11)</f>
+        <f>IF(G3&lt;=F3, 0, G3-F3)</f>
         <v>0</v>
       </c>
       <c r="I3" s="2">
         <v>10</v>
       </c>
       <c r="J3" s="2">
-        <f>H3*I3</f>
+        <f>I3*H3</f>
         <v>0</v>
       </c>
       <c r="K3" s="2">
-        <f>E3+J3</f>
+        <f>SUM(E3+J3)</f>
         <v>1694.0000000000002</v>
       </c>
       <c r="L3" s="1"/>
@@ -783,10 +789,11 @@
         <f>A3+1</f>
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>22</v>
+      <c r="B4" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="C4" s="2">
+        <f>C3-0.5</f>
         <v>69.5</v>
       </c>
       <c r="D4" s="2">
@@ -794,28 +801,31 @@
         <v>24.200000000000003</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" ref="E4:E38" si="1">C4*D4</f>
+        <f t="shared" ref="E4:E38" si="1">D4*C4</f>
         <v>1681.9</v>
       </c>
       <c r="F4" s="4">
+        <f>$F$3</f>
         <v>44813</v>
       </c>
       <c r="G4" s="4">
+        <f>G3+1</f>
         <v>44806</v>
       </c>
       <c r="H4" s="2">
-        <f t="shared" ref="H4:H38" si="2">IF(G4&lt;=F4,0,A4-$A$11)</f>
+        <f>IF(G4&lt;=F4, 0, G4-F4)</f>
         <v>0</v>
       </c>
       <c r="I4" s="2">
+        <f>$I$3</f>
         <v>10</v>
       </c>
       <c r="J4" s="2">
-        <f t="shared" ref="J4:J38" si="3">H4*I4</f>
+        <f t="shared" ref="J4:J38" si="2">I4*H4</f>
         <v>0</v>
       </c>
       <c r="K4" s="2">
-        <f t="shared" ref="K4:K38" si="4">E4+J4</f>
+        <f t="shared" ref="K4:K38" si="3">SUM(E4+J4)</f>
         <v>1681.9</v>
       </c>
       <c r="L4" s="1"/>
@@ -866,13 +876,14 @@
     </row>
     <row r="5" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <f t="shared" ref="A5:A38" si="5">A4+1</f>
+        <f t="shared" ref="A5:A38" si="4">A4+1</f>
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>24</v>
+      <c r="B5" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="C5" s="2">
+        <f t="shared" ref="C5:C38" si="5">C4-0.5</f>
         <v>69</v>
       </c>
       <c r="D5" s="2">
@@ -884,24 +895,27 @@
         <v>1669.8000000000002</v>
       </c>
       <c r="F5" s="4">
+        <f t="shared" ref="F5:F38" si="6">$F$3</f>
         <v>44813</v>
       </c>
       <c r="G5" s="4">
+        <f t="shared" ref="G5:G38" si="7">G4+1</f>
         <v>44807</v>
       </c>
       <c r="H5" s="2">
+        <f t="shared" ref="H5:H38" si="8">IF(G5&lt;=F5, 0, G5-F5)</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" ref="I5:I38" si="9">$I$3</f>
+        <v>10</v>
+      </c>
+      <c r="J5" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I5" s="2">
-        <v>10</v>
-      </c>
-      <c r="J5" s="2">
+      <c r="K5" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K5" s="2">
-        <f t="shared" si="4"/>
         <v>1669.8000000000002</v>
       </c>
       <c r="L5" s="1"/>
@@ -952,13 +966,14 @@
     </row>
     <row r="6" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2">
         <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="2">
         <v>68.5</v>
       </c>
       <c r="D6" s="2">
@@ -970,24 +985,27 @@
         <v>1657.7000000000003</v>
       </c>
       <c r="F6" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G6" s="4">
+        <f t="shared" si="7"/>
         <v>44808</v>
       </c>
       <c r="H6" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J6" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I6" s="2">
-        <v>10</v>
-      </c>
-      <c r="J6" s="2">
+      <c r="K6" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K6" s="2">
-        <f t="shared" si="4"/>
         <v>1657.7000000000003</v>
       </c>
       <c r="L6" s="1"/>
@@ -1038,13 +1056,14 @@
     </row>
     <row r="7" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="2">
         <v>68</v>
       </c>
       <c r="D7" s="2">
@@ -1056,24 +1075,27 @@
         <v>1645.6000000000001</v>
       </c>
       <c r="F7" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G7" s="4">
+        <f t="shared" si="7"/>
         <v>44809</v>
       </c>
       <c r="H7" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J7" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I7" s="2">
-        <v>10</v>
-      </c>
-      <c r="J7" s="2">
+      <c r="K7" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K7" s="2">
-        <f t="shared" si="4"/>
         <v>1645.6000000000001</v>
       </c>
       <c r="L7" s="1"/>
@@ -1124,13 +1146,14 @@
     </row>
     <row r="8" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2">
         <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="2">
         <v>67.5</v>
       </c>
       <c r="D8" s="2">
@@ -1142,24 +1165,27 @@
         <v>1633.5000000000002</v>
       </c>
       <c r="F8" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G8" s="4">
+        <f t="shared" si="7"/>
         <v>44810</v>
       </c>
       <c r="H8" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J8" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I8" s="2">
-        <v>10</v>
-      </c>
-      <c r="J8" s="2">
+      <c r="K8" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K8" s="2">
-        <f t="shared" si="4"/>
         <v>1633.5000000000002</v>
       </c>
       <c r="L8" s="1"/>
@@ -1210,13 +1236,14 @@
     </row>
     <row r="9" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="2">
         <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="2">
         <v>67</v>
       </c>
       <c r="D9" s="2">
@@ -1228,24 +1255,27 @@
         <v>1621.4</v>
       </c>
       <c r="F9" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G9" s="4">
+        <f t="shared" si="7"/>
         <v>44811</v>
       </c>
       <c r="H9" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J9" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I9" s="2">
-        <v>10</v>
-      </c>
-      <c r="J9" s="2">
+      <c r="K9" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K9" s="2">
-        <f t="shared" si="4"/>
         <v>1621.4</v>
       </c>
       <c r="L9" s="1"/>
@@ -1296,13 +1326,14 @@
     </row>
     <row r="10" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="2">
         <v>66.5</v>
       </c>
       <c r="D10" s="2">
@@ -1314,24 +1345,27 @@
         <v>1609.3000000000002</v>
       </c>
       <c r="F10" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G10" s="4">
+        <f t="shared" si="7"/>
         <v>44812</v>
       </c>
       <c r="H10" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J10" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I10" s="2">
-        <v>10</v>
-      </c>
-      <c r="J10" s="2">
+      <c r="K10" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K10" s="2">
-        <f t="shared" si="4"/>
         <v>1609.3000000000002</v>
       </c>
       <c r="L10" s="1"/>
@@ -1382,13 +1416,14 @@
     </row>
     <row r="11" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="2">
         <f t="shared" si="5"/>
-        <v>9</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="2">
         <v>66</v>
       </c>
       <c r="D11" s="2">
@@ -1400,24 +1435,27 @@
         <v>1597.2000000000003</v>
       </c>
       <c r="F11" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G11" s="4">
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="H11" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J11" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I11" s="2">
-        <v>10</v>
-      </c>
-      <c r="J11" s="2">
+      <c r="K11" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K11" s="2">
-        <f t="shared" si="4"/>
         <v>1597.2000000000003</v>
       </c>
       <c r="L11" s="1"/>
@@ -1468,13 +1506,14 @@
     </row>
     <row r="12" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="2">
         <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="2">
         <v>65.5</v>
       </c>
       <c r="D12" s="2">
@@ -1486,24 +1525,27 @@
         <v>1585.1000000000001</v>
       </c>
       <c r="F12" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G12" s="4">
+        <f t="shared" si="7"/>
         <v>44814</v>
       </c>
       <c r="H12" s="2">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J12" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="I12" s="2">
         <v>10</v>
       </c>
-      <c r="J12" s="2">
+      <c r="K12" s="2">
         <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="K12" s="2">
-        <f t="shared" si="4"/>
         <v>1595.1000000000001</v>
       </c>
       <c r="L12" s="1"/>
@@ -1554,13 +1596,14 @@
     </row>
     <row r="13" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="2">
         <f t="shared" si="5"/>
-        <v>11</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="2">
         <v>65</v>
       </c>
       <c r="D13" s="2">
@@ -1572,24 +1615,27 @@
         <v>1573.0000000000002</v>
       </c>
       <c r="F13" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G13" s="4">
+        <f t="shared" si="7"/>
         <v>44815</v>
       </c>
       <c r="H13" s="2">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J13" s="2">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="I13" s="2">
-        <v>10</v>
-      </c>
-      <c r="J13" s="2">
+        <v>20</v>
+      </c>
+      <c r="K13" s="2">
         <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="K13" s="2">
-        <f t="shared" si="4"/>
         <v>1593.0000000000002</v>
       </c>
       <c r="L13" s="1"/>
@@ -1640,13 +1686,14 @@
     </row>
     <row r="14" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="2">
         <f t="shared" si="5"/>
-        <v>12</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="2">
         <v>64.5</v>
       </c>
       <c r="D14" s="2">
@@ -1658,24 +1705,27 @@
         <v>1560.9</v>
       </c>
       <c r="F14" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G14" s="4">
+        <f t="shared" si="7"/>
         <v>44816</v>
       </c>
       <c r="H14" s="2">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J14" s="2">
         <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="I14" s="2">
-        <v>10</v>
-      </c>
-      <c r="J14" s="2">
+        <v>30</v>
+      </c>
+      <c r="K14" s="2">
         <f t="shared" si="3"/>
-        <v>30</v>
-      </c>
-      <c r="K14" s="2">
-        <f t="shared" si="4"/>
         <v>1590.9</v>
       </c>
       <c r="L14" s="1"/>
@@ -1726,13 +1776,14 @@
     </row>
     <row r="15" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="2">
         <f t="shared" si="5"/>
-        <v>13</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="2">
         <v>64</v>
       </c>
       <c r="D15" s="2">
@@ -1744,24 +1795,27 @@
         <v>1548.8000000000002</v>
       </c>
       <c r="F15" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G15" s="4">
+        <f t="shared" si="7"/>
         <v>44817</v>
       </c>
       <c r="H15" s="2">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J15" s="2">
         <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="I15" s="2">
-        <v>10</v>
-      </c>
-      <c r="J15" s="2">
+        <v>40</v>
+      </c>
+      <c r="K15" s="2">
         <f t="shared" si="3"/>
-        <v>40</v>
-      </c>
-      <c r="K15" s="2">
-        <f t="shared" si="4"/>
         <v>1588.8000000000002</v>
       </c>
       <c r="L15" s="1"/>
@@ -1812,13 +1866,14 @@
     </row>
     <row r="16" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="2">
         <f t="shared" si="5"/>
-        <v>14</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="2">
         <v>63.5</v>
       </c>
       <c r="D16" s="2">
@@ -1830,24 +1885,27 @@
         <v>1536.7000000000003</v>
       </c>
       <c r="F16" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G16" s="4">
+        <f t="shared" si="7"/>
         <v>44818</v>
       </c>
       <c r="H16" s="2">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J16" s="2">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="I16" s="2">
-        <v>10</v>
-      </c>
-      <c r="J16" s="2">
+        <v>50</v>
+      </c>
+      <c r="K16" s="2">
         <f t="shared" si="3"/>
-        <v>50</v>
-      </c>
-      <c r="K16" s="2">
-        <f t="shared" si="4"/>
         <v>1586.7000000000003</v>
       </c>
       <c r="L16" s="1"/>
@@ -1898,13 +1956,14 @@
     </row>
     <row r="17" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="2">
         <f t="shared" si="5"/>
-        <v>15</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="2">
         <v>63</v>
       </c>
       <c r="D17" s="2">
@@ -1916,24 +1975,27 @@
         <v>1524.6000000000001</v>
       </c>
       <c r="F17" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G17" s="4">
+        <f t="shared" si="7"/>
         <v>44819</v>
       </c>
       <c r="H17" s="2">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J17" s="2">
         <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="I17" s="2">
-        <v>10</v>
-      </c>
-      <c r="J17" s="2">
+        <v>60</v>
+      </c>
+      <c r="K17" s="2">
         <f t="shared" si="3"/>
-        <v>60</v>
-      </c>
-      <c r="K17" s="2">
-        <f t="shared" si="4"/>
         <v>1584.6000000000001</v>
       </c>
       <c r="L17" s="1"/>
@@ -1984,13 +2046,14 @@
     </row>
     <row r="18" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="2">
         <f t="shared" si="5"/>
-        <v>16</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="2">
         <v>62.5</v>
       </c>
       <c r="D18" s="2">
@@ -2002,24 +2065,27 @@
         <v>1512.5000000000002</v>
       </c>
       <c r="F18" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G18" s="4">
+        <f t="shared" si="7"/>
         <v>44820</v>
       </c>
       <c r="H18" s="2">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J18" s="2">
         <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="I18" s="2">
-        <v>10</v>
-      </c>
-      <c r="J18" s="2">
+        <v>70</v>
+      </c>
+      <c r="K18" s="2">
         <f t="shared" si="3"/>
-        <v>70</v>
-      </c>
-      <c r="K18" s="2">
-        <f t="shared" si="4"/>
         <v>1582.5000000000002</v>
       </c>
       <c r="L18" s="1"/>
@@ -2070,13 +2136,14 @@
     </row>
     <row r="19" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="2">
         <f t="shared" si="5"/>
-        <v>17</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="2">
         <v>62</v>
       </c>
       <c r="D19" s="2">
@@ -2088,24 +2155,27 @@
         <v>1500.4</v>
       </c>
       <c r="F19" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G19" s="4">
+        <f t="shared" si="7"/>
         <v>44821</v>
       </c>
       <c r="H19" s="2">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J19" s="2">
         <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="I19" s="2">
-        <v>10</v>
-      </c>
-      <c r="J19" s="2">
+        <v>80</v>
+      </c>
+      <c r="K19" s="2">
         <f t="shared" si="3"/>
-        <v>80</v>
-      </c>
-      <c r="K19" s="2">
-        <f t="shared" si="4"/>
         <v>1580.4</v>
       </c>
       <c r="L19" s="1"/>
@@ -2156,13 +2226,14 @@
     </row>
     <row r="20" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="2">
         <f t="shared" si="5"/>
-        <v>18</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="2">
         <v>61.5</v>
       </c>
       <c r="D20" s="2">
@@ -2174,24 +2245,27 @@
         <v>1488.3000000000002</v>
       </c>
       <c r="F20" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G20" s="4">
+        <f t="shared" si="7"/>
         <v>44822</v>
       </c>
       <c r="H20" s="2">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J20" s="2">
         <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="I20" s="2">
-        <v>10</v>
-      </c>
-      <c r="J20" s="2">
+        <v>90</v>
+      </c>
+      <c r="K20" s="2">
         <f t="shared" si="3"/>
-        <v>90</v>
-      </c>
-      <c r="K20" s="2">
-        <f t="shared" si="4"/>
         <v>1578.3000000000002</v>
       </c>
       <c r="L20" s="1"/>
@@ -2242,13 +2316,14 @@
     </row>
     <row r="21" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="2">
         <f t="shared" si="5"/>
-        <v>19</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="2">
         <v>61</v>
       </c>
       <c r="D21" s="2">
@@ -2260,24 +2335,27 @@
         <v>1476.2000000000003</v>
       </c>
       <c r="F21" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G21" s="4">
+        <f t="shared" si="7"/>
         <v>44823</v>
       </c>
       <c r="H21" s="2">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J21" s="2">
         <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="I21" s="2">
-        <v>10</v>
-      </c>
-      <c r="J21" s="2">
+        <v>100</v>
+      </c>
+      <c r="K21" s="2">
         <f t="shared" si="3"/>
-        <v>100</v>
-      </c>
-      <c r="K21" s="2">
-        <f t="shared" si="4"/>
         <v>1576.2000000000003</v>
       </c>
       <c r="L21" s="1"/>
@@ -2328,13 +2406,14 @@
     </row>
     <row r="22" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="2">
         <f t="shared" si="5"/>
-        <v>20</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="2">
         <v>60.5</v>
       </c>
       <c r="D22" s="2">
@@ -2346,24 +2425,27 @@
         <v>1464.1000000000001</v>
       </c>
       <c r="F22" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G22" s="4">
+        <f t="shared" si="7"/>
         <v>44824</v>
       </c>
       <c r="H22" s="2">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+      <c r="I22" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J22" s="2">
         <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-      <c r="I22" s="2">
-        <v>10</v>
-      </c>
-      <c r="J22" s="2">
+        <v>110</v>
+      </c>
+      <c r="K22" s="2">
         <f t="shared" si="3"/>
-        <v>110</v>
-      </c>
-      <c r="K22" s="2">
-        <f t="shared" si="4"/>
         <v>1574.1000000000001</v>
       </c>
       <c r="L22" s="1"/>
@@ -2414,13 +2496,14 @@
     </row>
     <row r="23" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2">
         <f t="shared" si="5"/>
-        <v>21</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="2">
         <v>60</v>
       </c>
       <c r="D23" s="2">
@@ -2432,24 +2515,27 @@
         <v>1452.0000000000002</v>
       </c>
       <c r="F23" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G23" s="4">
+        <f t="shared" si="7"/>
         <v>44825</v>
       </c>
       <c r="H23" s="2">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+      <c r="I23" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J23" s="2">
         <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="I23" s="2">
-        <v>10</v>
-      </c>
-      <c r="J23" s="2">
+        <v>120</v>
+      </c>
+      <c r="K23" s="2">
         <f t="shared" si="3"/>
-        <v>120</v>
-      </c>
-      <c r="K23" s="2">
-        <f t="shared" si="4"/>
         <v>1572.0000000000002</v>
       </c>
       <c r="L23" s="1"/>
@@ -2500,13 +2586,14 @@
     </row>
     <row r="24" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="2">
         <f t="shared" si="5"/>
-        <v>22</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="2">
         <v>59.5</v>
       </c>
       <c r="D24" s="2">
@@ -2518,24 +2605,27 @@
         <v>1439.9</v>
       </c>
       <c r="F24" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G24" s="4">
+        <f t="shared" si="7"/>
         <v>44826</v>
       </c>
       <c r="H24" s="2">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+      <c r="I24" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J24" s="2">
         <f t="shared" si="2"/>
-        <v>13</v>
-      </c>
-      <c r="I24" s="2">
-        <v>10</v>
-      </c>
-      <c r="J24" s="2">
+        <v>130</v>
+      </c>
+      <c r="K24" s="2">
         <f t="shared" si="3"/>
-        <v>130</v>
-      </c>
-      <c r="K24" s="2">
-        <f t="shared" si="4"/>
         <v>1569.9</v>
       </c>
       <c r="L24" s="1"/>
@@ -2586,13 +2676,14 @@
     </row>
     <row r="25" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="2">
         <f t="shared" si="5"/>
-        <v>23</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="2">
         <v>59</v>
       </c>
       <c r="D25" s="2">
@@ -2604,24 +2695,27 @@
         <v>1427.8000000000002</v>
       </c>
       <c r="F25" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G25" s="4">
+        <f t="shared" si="7"/>
         <v>44827</v>
       </c>
       <c r="H25" s="2">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+      <c r="I25" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J25" s="2">
         <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="I25" s="2">
-        <v>10</v>
-      </c>
-      <c r="J25" s="2">
+        <v>140</v>
+      </c>
+      <c r="K25" s="2">
         <f t="shared" si="3"/>
-        <v>140</v>
-      </c>
-      <c r="K25" s="2">
-        <f t="shared" si="4"/>
         <v>1567.8000000000002</v>
       </c>
       <c r="L25" s="1"/>
@@ -2672,13 +2766,14 @@
     </row>
     <row r="26" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="2">
         <f t="shared" si="5"/>
-        <v>24</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="2">
         <v>58.5</v>
       </c>
       <c r="D26" s="2">
@@ -2690,24 +2785,27 @@
         <v>1415.7000000000003</v>
       </c>
       <c r="F26" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G26" s="4">
+        <f t="shared" si="7"/>
         <v>44828</v>
       </c>
       <c r="H26" s="2">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J26" s="2">
         <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="I26" s="2">
-        <v>10</v>
-      </c>
-      <c r="J26" s="2">
+        <v>150</v>
+      </c>
+      <c r="K26" s="2">
         <f t="shared" si="3"/>
-        <v>150</v>
-      </c>
-      <c r="K26" s="2">
-        <f t="shared" si="4"/>
         <v>1565.7000000000003</v>
       </c>
       <c r="L26" s="1"/>
@@ -2758,13 +2856,14 @@
     </row>
     <row r="27" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="2">
         <f t="shared" si="5"/>
-        <v>25</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="2">
         <v>58</v>
       </c>
       <c r="D27" s="2">
@@ -2776,24 +2875,27 @@
         <v>1403.6000000000001</v>
       </c>
       <c r="F27" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G27" s="4">
+        <f t="shared" si="7"/>
         <v>44829</v>
       </c>
       <c r="H27" s="2">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+      <c r="I27" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J27" s="2">
         <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="I27" s="2">
-        <v>10</v>
-      </c>
-      <c r="J27" s="2">
+        <v>160</v>
+      </c>
+      <c r="K27" s="2">
         <f t="shared" si="3"/>
-        <v>160</v>
-      </c>
-      <c r="K27" s="2">
-        <f t="shared" si="4"/>
         <v>1563.6000000000001</v>
       </c>
       <c r="L27" s="1"/>
@@ -2844,13 +2946,14 @@
     </row>
     <row r="28" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="2">
         <f t="shared" si="5"/>
-        <v>26</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="2">
         <v>57.5</v>
       </c>
       <c r="D28" s="2">
@@ -2862,24 +2965,27 @@
         <v>1391.5000000000002</v>
       </c>
       <c r="F28" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G28" s="4">
+        <f t="shared" si="7"/>
         <v>44830</v>
       </c>
       <c r="H28" s="2">
+        <f t="shared" si="8"/>
+        <v>17</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J28" s="2">
         <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
-      <c r="I28" s="2">
-        <v>10</v>
-      </c>
-      <c r="J28" s="2">
+        <v>170</v>
+      </c>
+      <c r="K28" s="2">
         <f t="shared" si="3"/>
-        <v>170</v>
-      </c>
-      <c r="K28" s="2">
-        <f t="shared" si="4"/>
         <v>1561.5000000000002</v>
       </c>
       <c r="L28" s="1"/>
@@ -2930,13 +3036,14 @@
     </row>
     <row r="29" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
+        <f t="shared" si="4"/>
+        <v>27</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="2">
         <f t="shared" si="5"/>
-        <v>27</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="2">
         <v>57</v>
       </c>
       <c r="D29" s="2">
@@ -2948,24 +3055,27 @@
         <v>1379.4</v>
       </c>
       <c r="F29" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G29" s="4">
+        <f t="shared" si="7"/>
         <v>44831</v>
       </c>
       <c r="H29" s="2">
+        <f t="shared" si="8"/>
+        <v>18</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J29" s="2">
         <f t="shared" si="2"/>
-        <v>18</v>
-      </c>
-      <c r="I29" s="2">
-        <v>10</v>
-      </c>
-      <c r="J29" s="2">
+        <v>180</v>
+      </c>
+      <c r="K29" s="2">
         <f t="shared" si="3"/>
-        <v>180</v>
-      </c>
-      <c r="K29" s="2">
-        <f t="shared" si="4"/>
         <v>1559.4</v>
       </c>
       <c r="L29" s="1"/>
@@ -3016,13 +3126,14 @@
     </row>
     <row r="30" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="2">
         <f t="shared" si="5"/>
-        <v>28</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C30" s="2">
         <v>56.5</v>
       </c>
       <c r="D30" s="2">
@@ -3034,24 +3145,27 @@
         <v>1367.3000000000002</v>
       </c>
       <c r="F30" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G30" s="4">
+        <f t="shared" si="7"/>
         <v>44832</v>
       </c>
       <c r="H30" s="2">
+        <f t="shared" si="8"/>
+        <v>19</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J30" s="2">
         <f t="shared" si="2"/>
-        <v>19</v>
-      </c>
-      <c r="I30" s="2">
-        <v>10</v>
-      </c>
-      <c r="J30" s="2">
+        <v>190</v>
+      </c>
+      <c r="K30" s="2">
         <f t="shared" si="3"/>
-        <v>190</v>
-      </c>
-      <c r="K30" s="2">
-        <f t="shared" si="4"/>
         <v>1557.3000000000002</v>
       </c>
       <c r="L30" s="1"/>
@@ -3102,13 +3216,14 @@
     </row>
     <row r="31" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="2">
         <f t="shared" si="5"/>
-        <v>29</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" s="2">
         <v>56</v>
       </c>
       <c r="D31" s="2">
@@ -3120,24 +3235,27 @@
         <v>1355.2000000000003</v>
       </c>
       <c r="F31" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G31" s="4">
+        <f t="shared" si="7"/>
         <v>44833</v>
       </c>
       <c r="H31" s="2">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J31" s="2">
         <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="I31" s="2">
-        <v>10</v>
-      </c>
-      <c r="J31" s="2">
+        <v>200</v>
+      </c>
+      <c r="K31" s="2">
         <f t="shared" si="3"/>
-        <v>200</v>
-      </c>
-      <c r="K31" s="2">
-        <f t="shared" si="4"/>
         <v>1555.2000000000003</v>
       </c>
       <c r="L31" s="1"/>
@@ -3188,13 +3306,14 @@
     </row>
     <row r="32" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="2">
         <f t="shared" si="5"/>
-        <v>30</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" s="2">
         <v>55.5</v>
       </c>
       <c r="D32" s="2">
@@ -3206,24 +3325,27 @@
         <v>1343.1000000000001</v>
       </c>
       <c r="F32" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G32" s="4">
+        <f t="shared" si="7"/>
         <v>44834</v>
       </c>
       <c r="H32" s="2">
+        <f t="shared" si="8"/>
+        <v>21</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J32" s="2">
         <f t="shared" si="2"/>
-        <v>21</v>
-      </c>
-      <c r="I32" s="2">
-        <v>10</v>
-      </c>
-      <c r="J32" s="2">
+        <v>210</v>
+      </c>
+      <c r="K32" s="2">
         <f t="shared" si="3"/>
-        <v>210</v>
-      </c>
-      <c r="K32" s="2">
-        <f t="shared" si="4"/>
         <v>1553.1000000000001</v>
       </c>
       <c r="L32" s="1"/>
@@ -3274,13 +3396,14 @@
     </row>
     <row r="33" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="2">
         <f t="shared" si="5"/>
-        <v>31</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" s="2">
         <v>55</v>
       </c>
       <c r="D33" s="2">
@@ -3292,24 +3415,27 @@
         <v>1331.0000000000002</v>
       </c>
       <c r="F33" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G33" s="4">
+        <f t="shared" si="7"/>
         <v>44835</v>
       </c>
       <c r="H33" s="2">
+        <f t="shared" si="8"/>
+        <v>22</v>
+      </c>
+      <c r="I33" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J33" s="2">
         <f t="shared" si="2"/>
-        <v>22</v>
-      </c>
-      <c r="I33" s="2">
-        <v>10</v>
-      </c>
-      <c r="J33" s="2">
+        <v>220</v>
+      </c>
+      <c r="K33" s="2">
         <f t="shared" si="3"/>
-        <v>220</v>
-      </c>
-      <c r="K33" s="2">
-        <f t="shared" si="4"/>
         <v>1551.0000000000002</v>
       </c>
       <c r="L33" s="1"/>
@@ -3360,13 +3486,14 @@
     </row>
     <row r="34" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="2">
         <f t="shared" si="5"/>
-        <v>32</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" s="2">
         <v>54.5</v>
       </c>
       <c r="D34" s="2">
@@ -3378,24 +3505,27 @@
         <v>1318.9</v>
       </c>
       <c r="F34" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G34" s="4">
+        <f t="shared" si="7"/>
         <v>44836</v>
       </c>
       <c r="H34" s="2">
+        <f t="shared" si="8"/>
+        <v>23</v>
+      </c>
+      <c r="I34" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J34" s="2">
         <f t="shared" si="2"/>
-        <v>23</v>
-      </c>
-      <c r="I34" s="2">
-        <v>10</v>
-      </c>
-      <c r="J34" s="2">
+        <v>230</v>
+      </c>
+      <c r="K34" s="2">
         <f t="shared" si="3"/>
-        <v>230</v>
-      </c>
-      <c r="K34" s="2">
-        <f t="shared" si="4"/>
         <v>1548.9</v>
       </c>
       <c r="L34" s="1"/>
@@ -3446,13 +3576,14 @@
     </row>
     <row r="35" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
+        <f t="shared" si="4"/>
+        <v>33</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="2">
         <f t="shared" si="5"/>
-        <v>33</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C35" s="2">
         <v>54</v>
       </c>
       <c r="D35" s="2">
@@ -3464,24 +3595,27 @@
         <v>653.40000000000009</v>
       </c>
       <c r="F35" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G35" s="4">
+        <f t="shared" si="7"/>
         <v>44837</v>
       </c>
       <c r="H35" s="2">
+        <f t="shared" si="8"/>
+        <v>24</v>
+      </c>
+      <c r="I35" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J35" s="2">
         <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="I35" s="2">
-        <v>10</v>
-      </c>
-      <c r="J35" s="2">
+        <v>240</v>
+      </c>
+      <c r="K35" s="2">
         <f t="shared" si="3"/>
-        <v>240</v>
-      </c>
-      <c r="K35" s="2">
-        <f t="shared" si="4"/>
         <v>893.40000000000009</v>
       </c>
       <c r="L35" s="1"/>
@@ -3532,17 +3666,18 @@
     </row>
     <row r="36" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
+        <f t="shared" si="4"/>
+        <v>34</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="2">
         <f t="shared" si="5"/>
-        <v>34</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C36" s="2">
         <v>53.5</v>
       </c>
       <c r="D36" s="2">
-        <f t="shared" ref="D36:D38" si="6">22*1.1/2</f>
+        <f t="shared" ref="D36:D38" si="10">22*1.1/2</f>
         <v>12.100000000000001</v>
       </c>
       <c r="E36" s="2">
@@ -3550,24 +3685,27 @@
         <v>647.35</v>
       </c>
       <c r="F36" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G36" s="4">
+        <f t="shared" si="7"/>
         <v>44838</v>
       </c>
       <c r="H36" s="2">
+        <f t="shared" si="8"/>
+        <v>25</v>
+      </c>
+      <c r="I36" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J36" s="2">
         <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-      <c r="I36" s="2">
-        <v>10</v>
-      </c>
-      <c r="J36" s="2">
+        <v>250</v>
+      </c>
+      <c r="K36" s="2">
         <f t="shared" si="3"/>
-        <v>250</v>
-      </c>
-      <c r="K36" s="2">
-        <f t="shared" si="4"/>
         <v>897.35</v>
       </c>
       <c r="L36" s="1"/>
@@ -3618,17 +3756,18 @@
     </row>
     <row r="37" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
+        <f t="shared" si="4"/>
+        <v>35</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="2">
         <f t="shared" si="5"/>
-        <v>35</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C37" s="2">
         <v>53</v>
       </c>
       <c r="D37" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>12.100000000000001</v>
       </c>
       <c r="E37" s="2">
@@ -3636,24 +3775,27 @@
         <v>641.30000000000007</v>
       </c>
       <c r="F37" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G37" s="4">
+        <f t="shared" si="7"/>
         <v>44839</v>
       </c>
       <c r="H37" s="2">
+        <f t="shared" si="8"/>
+        <v>26</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J37" s="2">
         <f t="shared" si="2"/>
-        <v>26</v>
-      </c>
-      <c r="I37" s="2">
-        <v>10</v>
-      </c>
-      <c r="J37" s="2">
+        <v>260</v>
+      </c>
+      <c r="K37" s="2">
         <f t="shared" si="3"/>
-        <v>260</v>
-      </c>
-      <c r="K37" s="2">
-        <f t="shared" si="4"/>
         <v>901.30000000000007</v>
       </c>
       <c r="L37" s="1"/>
@@ -3704,17 +3846,18 @@
     </row>
     <row r="38" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
+        <f t="shared" si="4"/>
+        <v>36</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" s="2">
         <f t="shared" si="5"/>
-        <v>36</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C38" s="2">
         <v>52.5</v>
       </c>
       <c r="D38" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>12.100000000000001</v>
       </c>
       <c r="E38" s="2">
@@ -3722,24 +3865,27 @@
         <v>635.25000000000011</v>
       </c>
       <c r="F38" s="4">
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G38" s="4">
+        <f t="shared" si="7"/>
         <v>44840</v>
       </c>
       <c r="H38" s="2">
+        <f t="shared" si="8"/>
+        <v>27</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="J38" s="2">
         <f t="shared" si="2"/>
-        <v>27</v>
-      </c>
-      <c r="I38" s="2">
-        <v>10</v>
-      </c>
-      <c r="J38" s="2">
+        <v>270</v>
+      </c>
+      <c r="K38" s="2">
         <f t="shared" si="3"/>
-        <v>270</v>
-      </c>
-      <c r="K38" s="2">
-        <f t="shared" si="4"/>
         <v>905.25000000000011</v>
       </c>
       <c r="L38" s="1"/>
@@ -3849,7 +3995,7 @@
     <row r="40" spans="1:56" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C40" s="5">
         <f>SUM(K3:K38)</f>
@@ -3912,7 +4058,7 @@
     <row r="41" spans="1:56" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C41" s="2">
         <f>AVERAGE(C3:C38)</f>
@@ -3975,7 +4121,7 @@
     <row r="42" spans="1:56" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C42" s="2">
         <f>MAX(H3:H38)</f>
@@ -4038,7 +4184,7 @@
     <row r="43" spans="1:56" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C43" s="2">
         <f>MAX(K3:K38)</f>

</xml_diff>

<commit_message>
Sending 1_22_xlsx - try 6 ¯\_(ツ)_/¯
</commit_message>
<xml_diff>
--- a/LR3/table_1_22.xlsx
+++ b/LR3/table_1_22.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{52F15052-81F0-405E-AF9F-C03F2F2F9F15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{819CC67D-D9BA-4967-8540-47ADF0D7DB72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5484" yWindow="2172" windowWidth="18912" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2172" windowWidth="18912" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -165,18 +165,6 @@
     <t>Тариф, руб./кв.м.</t>
   </si>
   <si>
-    <t>средняя площадь, кв.м.</t>
-  </si>
-  <si>
-    <t>максимальный срок просрочки, дней</t>
-  </si>
-  <si>
-    <t>максимальная сумма к оплате, руб.</t>
-  </si>
-  <si>
-    <t>общая сумма графы "Итого", руб.</t>
-  </si>
-  <si>
     <t>Фамилия квартиросъёмщика</t>
   </si>
   <si>
@@ -184,6 +172,18 @@
   </si>
   <si>
     <t>Дата оплаты, день</t>
+  </si>
+  <si>
+    <t>Общая сумма, руб.</t>
+  </si>
+  <si>
+    <t>Средняя площадь, кв.м.</t>
+  </si>
+  <si>
+    <t>Максимальный срок просрочки, дней</t>
+  </si>
+  <si>
+    <t>Максимальная сумма, руб.</t>
   </si>
 </sst>
 </file>
@@ -543,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="57" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -624,7 +624,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>17</v>
@@ -636,10 +636,10 @@
         <v>38</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>42</v>
@@ -735,7 +735,7 @@
         <v>0</v>
       </c>
       <c r="K3" s="2">
-        <f>SUM(E3+J3)</f>
+        <f>SUM(E3,J3)</f>
         <v>1694.0000000000002</v>
       </c>
       <c r="L3" s="1"/>
@@ -797,11 +797,11 @@
         <v>69.5</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" ref="D4:D34" si="0">22*1.1</f>
+        <f>IF((A4 / 4 &lt;= 8),$D$3, $D$3/2)</f>
         <v>24.200000000000003</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" ref="E4:E38" si="1">D4*C4</f>
+        <f t="shared" ref="E4:E38" si="0">D4*C4</f>
         <v>1681.9</v>
       </c>
       <c r="F4" s="4">
@@ -821,11 +821,11 @@
         <v>10</v>
       </c>
       <c r="J4" s="2">
-        <f t="shared" ref="J4:J38" si="2">I4*H4</f>
+        <f t="shared" ref="J4:J38" si="1">I4*H4</f>
         <v>0</v>
       </c>
       <c r="K4" s="2">
-        <f t="shared" ref="K4:K38" si="3">SUM(E4+J4)</f>
+        <f t="shared" ref="K4:K38" si="2">SUM(E4,J4)</f>
         <v>1681.9</v>
       </c>
       <c r="L4" s="1"/>
@@ -876,22 +876,22 @@
     </row>
     <row r="5" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <f t="shared" ref="A5:A38" si="4">A4+1</f>
+        <f t="shared" ref="A5:A38" si="3">A4+1</f>
         <v>3</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="2">
-        <f t="shared" ref="C5:C38" si="5">C4-0.5</f>
+        <f t="shared" ref="C5:C38" si="4">C4-0.5</f>
         <v>69</v>
       </c>
       <c r="D5" s="2">
+        <f t="shared" ref="D5:D38" si="5">IF((A5 / 4 &lt;= 8),$D$3, $D$3/2)</f>
+        <v>24.200000000000003</v>
+      </c>
+      <c r="E5" s="2">
         <f t="shared" si="0"/>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="E5" s="2">
-        <f t="shared" si="1"/>
         <v>1669.8000000000002</v>
       </c>
       <c r="F5" s="4">
@@ -911,11 +911,11 @@
         <v>10</v>
       </c>
       <c r="J5" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K5" s="2">
-        <f t="shared" si="3"/>
         <v>1669.8000000000002</v>
       </c>
       <c r="L5" s="1"/>
@@ -966,22 +966,22 @@
     </row>
     <row r="6" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="2">
+        <f t="shared" si="4"/>
+        <v>68.5</v>
+      </c>
+      <c r="D6" s="2">
         <f t="shared" si="5"/>
-        <v>68.5</v>
-      </c>
-      <c r="D6" s="2">
+        <v>24.200000000000003</v>
+      </c>
+      <c r="E6" s="2">
         <f t="shared" si="0"/>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="E6" s="2">
-        <f t="shared" si="1"/>
         <v>1657.7000000000003</v>
       </c>
       <c r="F6" s="4">
@@ -1001,11 +1001,11 @@
         <v>10</v>
       </c>
       <c r="J6" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K6" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K6" s="2">
-        <f t="shared" si="3"/>
         <v>1657.7000000000003</v>
       </c>
       <c r="L6" s="1"/>
@@ -1056,22 +1056,22 @@
     </row>
     <row r="7" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="2">
+        <f t="shared" si="4"/>
+        <v>68</v>
+      </c>
+      <c r="D7" s="2">
         <f t="shared" si="5"/>
-        <v>68</v>
-      </c>
-      <c r="D7" s="2">
+        <v>24.200000000000003</v>
+      </c>
+      <c r="E7" s="2">
         <f t="shared" si="0"/>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="E7" s="2">
-        <f t="shared" si="1"/>
         <v>1645.6000000000001</v>
       </c>
       <c r="F7" s="4">
@@ -1091,11 +1091,11 @@
         <v>10</v>
       </c>
       <c r="J7" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K7" s="2">
-        <f t="shared" si="3"/>
         <v>1645.6000000000001</v>
       </c>
       <c r="L7" s="1"/>
@@ -1146,22 +1146,22 @@
     </row>
     <row r="8" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="2">
+        <f t="shared" si="4"/>
+        <v>67.5</v>
+      </c>
+      <c r="D8" s="2">
         <f t="shared" si="5"/>
-        <v>67.5</v>
-      </c>
-      <c r="D8" s="2">
+        <v>24.200000000000003</v>
+      </c>
+      <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="E8" s="2">
-        <f t="shared" si="1"/>
         <v>1633.5000000000002</v>
       </c>
       <c r="F8" s="4">
@@ -1181,11 +1181,11 @@
         <v>10</v>
       </c>
       <c r="J8" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K8" s="2">
-        <f t="shared" si="3"/>
         <v>1633.5000000000002</v>
       </c>
       <c r="L8" s="1"/>
@@ -1236,22 +1236,22 @@
     </row>
     <row r="9" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="2">
+        <f t="shared" si="4"/>
+        <v>67</v>
+      </c>
+      <c r="D9" s="2">
         <f t="shared" si="5"/>
-        <v>67</v>
-      </c>
-      <c r="D9" s="2">
+        <v>24.200000000000003</v>
+      </c>
+      <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="E9" s="2">
-        <f t="shared" si="1"/>
         <v>1621.4</v>
       </c>
       <c r="F9" s="4">
@@ -1271,11 +1271,11 @@
         <v>10</v>
       </c>
       <c r="J9" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K9" s="2">
-        <f t="shared" si="3"/>
         <v>1621.4</v>
       </c>
       <c r="L9" s="1"/>
@@ -1326,22 +1326,22 @@
     </row>
     <row r="10" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C10" s="2">
+        <f t="shared" si="4"/>
+        <v>66.5</v>
+      </c>
+      <c r="D10" s="2">
         <f t="shared" si="5"/>
-        <v>66.5</v>
-      </c>
-      <c r="D10" s="2">
+        <v>24.200000000000003</v>
+      </c>
+      <c r="E10" s="2">
         <f t="shared" si="0"/>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="E10" s="2">
-        <f t="shared" si="1"/>
         <v>1609.3000000000002</v>
       </c>
       <c r="F10" s="4">
@@ -1361,11 +1361,11 @@
         <v>10</v>
       </c>
       <c r="J10" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K10" s="2">
-        <f t="shared" si="3"/>
         <v>1609.3000000000002</v>
       </c>
       <c r="L10" s="1"/>
@@ -1416,22 +1416,22 @@
     </row>
     <row r="11" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C11" s="2">
+        <f t="shared" si="4"/>
+        <v>66</v>
+      </c>
+      <c r="D11" s="2">
         <f t="shared" si="5"/>
-        <v>66</v>
-      </c>
-      <c r="D11" s="2">
+        <v>24.200000000000003</v>
+      </c>
+      <c r="E11" s="2">
         <f t="shared" si="0"/>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="E11" s="2">
-        <f t="shared" si="1"/>
         <v>1597.2000000000003</v>
       </c>
       <c r="F11" s="4">
@@ -1451,11 +1451,11 @@
         <v>10</v>
       </c>
       <c r="J11" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K11" s="2">
-        <f t="shared" si="3"/>
         <v>1597.2000000000003</v>
       </c>
       <c r="L11" s="1"/>
@@ -1506,22 +1506,22 @@
     </row>
     <row r="12" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="2">
+        <f t="shared" si="4"/>
+        <v>65.5</v>
+      </c>
+      <c r="D12" s="2">
         <f t="shared" si="5"/>
-        <v>65.5</v>
-      </c>
-      <c r="D12" s="2">
+        <v>24.200000000000003</v>
+      </c>
+      <c r="E12" s="2">
         <f t="shared" si="0"/>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="E12" s="2">
-        <f t="shared" si="1"/>
         <v>1585.1000000000001</v>
       </c>
       <c r="F12" s="4">
@@ -1541,11 +1541,11 @@
         <v>10</v>
       </c>
       <c r="J12" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="K12" s="2">
         <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="K12" s="2">
-        <f t="shared" si="3"/>
         <v>1595.1000000000001</v>
       </c>
       <c r="L12" s="1"/>
@@ -1596,22 +1596,22 @@
     </row>
     <row r="13" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="2">
+        <f t="shared" si="4"/>
+        <v>65</v>
+      </c>
+      <c r="D13" s="2">
         <f t="shared" si="5"/>
-        <v>65</v>
-      </c>
-      <c r="D13" s="2">
+        <v>24.200000000000003</v>
+      </c>
+      <c r="E13" s="2">
         <f t="shared" si="0"/>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="E13" s="2">
-        <f t="shared" si="1"/>
         <v>1573.0000000000002</v>
       </c>
       <c r="F13" s="4">
@@ -1631,11 +1631,11 @@
         <v>10</v>
       </c>
       <c r="J13" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K13" s="2">
         <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="K13" s="2">
-        <f t="shared" si="3"/>
         <v>1593.0000000000002</v>
       </c>
       <c r="L13" s="1"/>
@@ -1686,22 +1686,22 @@
     </row>
     <row r="14" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="2">
+        <f t="shared" si="4"/>
+        <v>64.5</v>
+      </c>
+      <c r="D14" s="2">
         <f t="shared" si="5"/>
-        <v>64.5</v>
-      </c>
-      <c r="D14" s="2">
+        <v>24.200000000000003</v>
+      </c>
+      <c r="E14" s="2">
         <f t="shared" si="0"/>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="E14" s="2">
-        <f t="shared" si="1"/>
         <v>1560.9</v>
       </c>
       <c r="F14" s="4">
@@ -1721,11 +1721,11 @@
         <v>10</v>
       </c>
       <c r="J14" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="K14" s="2">
         <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="K14" s="2">
-        <f t="shared" si="3"/>
         <v>1590.9</v>
       </c>
       <c r="L14" s="1"/>
@@ -1776,22 +1776,22 @@
     </row>
     <row r="15" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="2">
+        <f t="shared" si="4"/>
+        <v>64</v>
+      </c>
+      <c r="D15" s="2">
         <f t="shared" si="5"/>
-        <v>64</v>
-      </c>
-      <c r="D15" s="2">
+        <v>24.200000000000003</v>
+      </c>
+      <c r="E15" s="2">
         <f t="shared" si="0"/>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="E15" s="2">
-        <f t="shared" si="1"/>
         <v>1548.8000000000002</v>
       </c>
       <c r="F15" s="4">
@@ -1811,11 +1811,11 @@
         <v>10</v>
       </c>
       <c r="J15" s="2">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="K15" s="2">
         <f t="shared" si="2"/>
-        <v>40</v>
-      </c>
-      <c r="K15" s="2">
-        <f t="shared" si="3"/>
         <v>1588.8000000000002</v>
       </c>
       <c r="L15" s="1"/>
@@ -1866,22 +1866,22 @@
     </row>
     <row r="16" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="2">
+        <f t="shared" si="4"/>
+        <v>63.5</v>
+      </c>
+      <c r="D16" s="2">
         <f t="shared" si="5"/>
-        <v>63.5</v>
-      </c>
-      <c r="D16" s="2">
+        <v>24.200000000000003</v>
+      </c>
+      <c r="E16" s="2">
         <f t="shared" si="0"/>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="E16" s="2">
-        <f t="shared" si="1"/>
         <v>1536.7000000000003</v>
       </c>
       <c r="F16" s="4">
@@ -1901,11 +1901,11 @@
         <v>10</v>
       </c>
       <c r="J16" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="K16" s="2">
         <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-      <c r="K16" s="2">
-        <f t="shared" si="3"/>
         <v>1586.7000000000003</v>
       </c>
       <c r="L16" s="1"/>
@@ -1956,22 +1956,22 @@
     </row>
     <row r="17" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C17" s="2">
+        <f t="shared" si="4"/>
+        <v>63</v>
+      </c>
+      <c r="D17" s="2">
         <f t="shared" si="5"/>
-        <v>63</v>
-      </c>
-      <c r="D17" s="2">
+        <v>24.200000000000003</v>
+      </c>
+      <c r="E17" s="2">
         <f t="shared" si="0"/>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="E17" s="2">
-        <f t="shared" si="1"/>
         <v>1524.6000000000001</v>
       </c>
       <c r="F17" s="4">
@@ -1991,11 +1991,11 @@
         <v>10</v>
       </c>
       <c r="J17" s="2">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="K17" s="2">
         <f t="shared" si="2"/>
-        <v>60</v>
-      </c>
-      <c r="K17" s="2">
-        <f t="shared" si="3"/>
         <v>1584.6000000000001</v>
       </c>
       <c r="L17" s="1"/>
@@ -2046,22 +2046,22 @@
     </row>
     <row r="18" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C18" s="2">
+        <f t="shared" si="4"/>
+        <v>62.5</v>
+      </c>
+      <c r="D18" s="2">
         <f t="shared" si="5"/>
-        <v>62.5</v>
-      </c>
-      <c r="D18" s="2">
+        <v>24.200000000000003</v>
+      </c>
+      <c r="E18" s="2">
         <f t="shared" si="0"/>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="E18" s="2">
-        <f t="shared" si="1"/>
         <v>1512.5000000000002</v>
       </c>
       <c r="F18" s="4">
@@ -2081,11 +2081,11 @@
         <v>10</v>
       </c>
       <c r="J18" s="2">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="K18" s="2">
         <f t="shared" si="2"/>
-        <v>70</v>
-      </c>
-      <c r="K18" s="2">
-        <f t="shared" si="3"/>
         <v>1582.5000000000002</v>
       </c>
       <c r="L18" s="1"/>
@@ -2136,22 +2136,22 @@
     </row>
     <row r="19" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>34</v>
       </c>
       <c r="C19" s="2">
+        <f t="shared" si="4"/>
+        <v>62</v>
+      </c>
+      <c r="D19" s="2">
         <f t="shared" si="5"/>
-        <v>62</v>
-      </c>
-      <c r="D19" s="2">
+        <v>24.200000000000003</v>
+      </c>
+      <c r="E19" s="2">
         <f t="shared" si="0"/>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="E19" s="2">
-        <f t="shared" si="1"/>
         <v>1500.4</v>
       </c>
       <c r="F19" s="4">
@@ -2171,11 +2171,11 @@
         <v>10</v>
       </c>
       <c r="J19" s="2">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="K19" s="2">
         <f t="shared" si="2"/>
-        <v>80</v>
-      </c>
-      <c r="K19" s="2">
-        <f t="shared" si="3"/>
         <v>1580.4</v>
       </c>
       <c r="L19" s="1"/>
@@ -2226,22 +2226,22 @@
     </row>
     <row r="20" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>36</v>
       </c>
       <c r="C20" s="2">
+        <f t="shared" si="4"/>
+        <v>61.5</v>
+      </c>
+      <c r="D20" s="2">
         <f t="shared" si="5"/>
-        <v>61.5</v>
-      </c>
-      <c r="D20" s="2">
+        <v>24.200000000000003</v>
+      </c>
+      <c r="E20" s="2">
         <f t="shared" si="0"/>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="E20" s="2">
-        <f t="shared" si="1"/>
         <v>1488.3000000000002</v>
       </c>
       <c r="F20" s="4">
@@ -2261,11 +2261,11 @@
         <v>10</v>
       </c>
       <c r="J20" s="2">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="K20" s="2">
         <f t="shared" si="2"/>
-        <v>90</v>
-      </c>
-      <c r="K20" s="2">
-        <f t="shared" si="3"/>
         <v>1578.3000000000002</v>
       </c>
       <c r="L20" s="1"/>
@@ -2316,22 +2316,22 @@
     </row>
     <row r="21" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C21" s="2">
+        <f t="shared" si="4"/>
+        <v>61</v>
+      </c>
+      <c r="D21" s="2">
         <f t="shared" si="5"/>
-        <v>61</v>
-      </c>
-      <c r="D21" s="2">
+        <v>24.200000000000003</v>
+      </c>
+      <c r="E21" s="2">
         <f t="shared" si="0"/>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="E21" s="2">
-        <f t="shared" si="1"/>
         <v>1476.2000000000003</v>
       </c>
       <c r="F21" s="4">
@@ -2351,11 +2351,11 @@
         <v>10</v>
       </c>
       <c r="J21" s="2">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="K21" s="2">
         <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-      <c r="K21" s="2">
-        <f t="shared" si="3"/>
         <v>1576.2000000000003</v>
       </c>
       <c r="L21" s="1"/>
@@ -2406,22 +2406,22 @@
     </row>
     <row r="22" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>37</v>
       </c>
       <c r="C22" s="2">
+        <f t="shared" si="4"/>
+        <v>60.5</v>
+      </c>
+      <c r="D22" s="2">
         <f t="shared" si="5"/>
-        <v>60.5</v>
-      </c>
-      <c r="D22" s="2">
+        <v>24.200000000000003</v>
+      </c>
+      <c r="E22" s="2">
         <f t="shared" si="0"/>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="E22" s="2">
-        <f t="shared" si="1"/>
         <v>1464.1000000000001</v>
       </c>
       <c r="F22" s="4">
@@ -2441,11 +2441,11 @@
         <v>10</v>
       </c>
       <c r="J22" s="2">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="K22" s="2">
         <f t="shared" si="2"/>
-        <v>110</v>
-      </c>
-      <c r="K22" s="2">
-        <f t="shared" si="3"/>
         <v>1574.1000000000001</v>
       </c>
       <c r="L22" s="1"/>
@@ -2496,22 +2496,22 @@
     </row>
     <row r="23" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="2">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+      <c r="D23" s="2">
         <f t="shared" si="5"/>
-        <v>60</v>
-      </c>
-      <c r="D23" s="2">
+        <v>24.200000000000003</v>
+      </c>
+      <c r="E23" s="2">
         <f t="shared" si="0"/>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="E23" s="2">
-        <f t="shared" si="1"/>
         <v>1452.0000000000002</v>
       </c>
       <c r="F23" s="4">
@@ -2531,11 +2531,11 @@
         <v>10</v>
       </c>
       <c r="J23" s="2">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="K23" s="2">
         <f t="shared" si="2"/>
-        <v>120</v>
-      </c>
-      <c r="K23" s="2">
-        <f t="shared" si="3"/>
         <v>1572.0000000000002</v>
       </c>
       <c r="L23" s="1"/>
@@ -2586,22 +2586,22 @@
     </row>
     <row r="24" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C24" s="2">
+        <f t="shared" si="4"/>
+        <v>59.5</v>
+      </c>
+      <c r="D24" s="2">
         <f t="shared" si="5"/>
-        <v>59.5</v>
-      </c>
-      <c r="D24" s="2">
+        <v>24.200000000000003</v>
+      </c>
+      <c r="E24" s="2">
         <f t="shared" si="0"/>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="E24" s="2">
-        <f t="shared" si="1"/>
         <v>1439.9</v>
       </c>
       <c r="F24" s="4">
@@ -2621,11 +2621,11 @@
         <v>10</v>
       </c>
       <c r="J24" s="2">
+        <f t="shared" si="1"/>
+        <v>130</v>
+      </c>
+      <c r="K24" s="2">
         <f t="shared" si="2"/>
-        <v>130</v>
-      </c>
-      <c r="K24" s="2">
-        <f t="shared" si="3"/>
         <v>1569.9</v>
       </c>
       <c r="L24" s="1"/>
@@ -2676,22 +2676,22 @@
     </row>
     <row r="25" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C25" s="2">
+        <f t="shared" si="4"/>
+        <v>59</v>
+      </c>
+      <c r="D25" s="2">
         <f t="shared" si="5"/>
-        <v>59</v>
-      </c>
-      <c r="D25" s="2">
+        <v>24.200000000000003</v>
+      </c>
+      <c r="E25" s="2">
         <f t="shared" si="0"/>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="E25" s="2">
-        <f t="shared" si="1"/>
         <v>1427.8000000000002</v>
       </c>
       <c r="F25" s="4">
@@ -2711,11 +2711,11 @@
         <v>10</v>
       </c>
       <c r="J25" s="2">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+      <c r="K25" s="2">
         <f t="shared" si="2"/>
-        <v>140</v>
-      </c>
-      <c r="K25" s="2">
-        <f t="shared" si="3"/>
         <v>1567.8000000000002</v>
       </c>
       <c r="L25" s="1"/>
@@ -2766,22 +2766,22 @@
     </row>
     <row r="26" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C26" s="2">
+        <f t="shared" si="4"/>
+        <v>58.5</v>
+      </c>
+      <c r="D26" s="2">
         <f t="shared" si="5"/>
-        <v>58.5</v>
-      </c>
-      <c r="D26" s="2">
+        <v>24.200000000000003</v>
+      </c>
+      <c r="E26" s="2">
         <f t="shared" si="0"/>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="E26" s="2">
-        <f t="shared" si="1"/>
         <v>1415.7000000000003</v>
       </c>
       <c r="F26" s="4">
@@ -2801,11 +2801,11 @@
         <v>10</v>
       </c>
       <c r="J26" s="2">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+      <c r="K26" s="2">
         <f t="shared" si="2"/>
-        <v>150</v>
-      </c>
-      <c r="K26" s="2">
-        <f t="shared" si="3"/>
         <v>1565.7000000000003</v>
       </c>
       <c r="L26" s="1"/>
@@ -2856,22 +2856,22 @@
     </row>
     <row r="27" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="2">
+        <f t="shared" si="4"/>
+        <v>58</v>
+      </c>
+      <c r="D27" s="2">
         <f t="shared" si="5"/>
-        <v>58</v>
-      </c>
-      <c r="D27" s="2">
+        <v>24.200000000000003</v>
+      </c>
+      <c r="E27" s="2">
         <f t="shared" si="0"/>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="E27" s="2">
-        <f t="shared" si="1"/>
         <v>1403.6000000000001</v>
       </c>
       <c r="F27" s="4">
@@ -2891,11 +2891,11 @@
         <v>10</v>
       </c>
       <c r="J27" s="2">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="K27" s="2">
         <f t="shared" si="2"/>
-        <v>160</v>
-      </c>
-      <c r="K27" s="2">
-        <f t="shared" si="3"/>
         <v>1563.6000000000001</v>
       </c>
       <c r="L27" s="1"/>
@@ -2946,22 +2946,22 @@
     </row>
     <row r="28" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C28" s="2">
+        <f t="shared" si="4"/>
+        <v>57.5</v>
+      </c>
+      <c r="D28" s="2">
         <f t="shared" si="5"/>
-        <v>57.5</v>
-      </c>
-      <c r="D28" s="2">
+        <v>24.200000000000003</v>
+      </c>
+      <c r="E28" s="2">
         <f t="shared" si="0"/>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="E28" s="2">
-        <f t="shared" si="1"/>
         <v>1391.5000000000002</v>
       </c>
       <c r="F28" s="4">
@@ -2981,11 +2981,11 @@
         <v>10</v>
       </c>
       <c r="J28" s="2">
+        <f t="shared" si="1"/>
+        <v>170</v>
+      </c>
+      <c r="K28" s="2">
         <f t="shared" si="2"/>
-        <v>170</v>
-      </c>
-      <c r="K28" s="2">
-        <f t="shared" si="3"/>
         <v>1561.5000000000002</v>
       </c>
       <c r="L28" s="1"/>
@@ -3036,22 +3036,22 @@
     </row>
     <row r="29" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C29" s="2">
+        <f t="shared" si="4"/>
+        <v>57</v>
+      </c>
+      <c r="D29" s="2">
         <f t="shared" si="5"/>
-        <v>57</v>
-      </c>
-      <c r="D29" s="2">
+        <v>24.200000000000003</v>
+      </c>
+      <c r="E29" s="2">
         <f t="shared" si="0"/>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="E29" s="2">
-        <f t="shared" si="1"/>
         <v>1379.4</v>
       </c>
       <c r="F29" s="4">
@@ -3071,11 +3071,11 @@
         <v>10</v>
       </c>
       <c r="J29" s="2">
+        <f t="shared" si="1"/>
+        <v>180</v>
+      </c>
+      <c r="K29" s="2">
         <f t="shared" si="2"/>
-        <v>180</v>
-      </c>
-      <c r="K29" s="2">
-        <f t="shared" si="3"/>
         <v>1559.4</v>
       </c>
       <c r="L29" s="1"/>
@@ -3126,22 +3126,22 @@
     </row>
     <row r="30" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C30" s="2">
+        <f t="shared" si="4"/>
+        <v>56.5</v>
+      </c>
+      <c r="D30" s="2">
         <f t="shared" si="5"/>
-        <v>56.5</v>
-      </c>
-      <c r="D30" s="2">
+        <v>24.200000000000003</v>
+      </c>
+      <c r="E30" s="2">
         <f t="shared" si="0"/>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="E30" s="2">
-        <f t="shared" si="1"/>
         <v>1367.3000000000002</v>
       </c>
       <c r="F30" s="4">
@@ -3161,11 +3161,11 @@
         <v>10</v>
       </c>
       <c r="J30" s="2">
+        <f t="shared" si="1"/>
+        <v>190</v>
+      </c>
+      <c r="K30" s="2">
         <f t="shared" si="2"/>
-        <v>190</v>
-      </c>
-      <c r="K30" s="2">
-        <f t="shared" si="3"/>
         <v>1557.3000000000002</v>
       </c>
       <c r="L30" s="1"/>
@@ -3216,22 +3216,22 @@
     </row>
     <row r="31" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>29</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C31" s="2">
+        <f t="shared" si="4"/>
+        <v>56</v>
+      </c>
+      <c r="D31" s="2">
         <f t="shared" si="5"/>
-        <v>56</v>
-      </c>
-      <c r="D31" s="2">
+        <v>24.200000000000003</v>
+      </c>
+      <c r="E31" s="2">
         <f t="shared" si="0"/>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="E31" s="2">
-        <f t="shared" si="1"/>
         <v>1355.2000000000003</v>
       </c>
       <c r="F31" s="4">
@@ -3251,11 +3251,11 @@
         <v>10</v>
       </c>
       <c r="J31" s="2">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="K31" s="2">
         <f t="shared" si="2"/>
-        <v>200</v>
-      </c>
-      <c r="K31" s="2">
-        <f t="shared" si="3"/>
         <v>1555.2000000000003</v>
       </c>
       <c r="L31" s="1"/>
@@ -3306,22 +3306,22 @@
     </row>
     <row r="32" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C32" s="2">
+        <f t="shared" si="4"/>
+        <v>55.5</v>
+      </c>
+      <c r="D32" s="2">
         <f t="shared" si="5"/>
-        <v>55.5</v>
-      </c>
-      <c r="D32" s="2">
+        <v>24.200000000000003</v>
+      </c>
+      <c r="E32" s="2">
         <f t="shared" si="0"/>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="E32" s="2">
-        <f t="shared" si="1"/>
         <v>1343.1000000000001</v>
       </c>
       <c r="F32" s="4">
@@ -3341,11 +3341,11 @@
         <v>10</v>
       </c>
       <c r="J32" s="2">
+        <f t="shared" si="1"/>
+        <v>210</v>
+      </c>
+      <c r="K32" s="2">
         <f t="shared" si="2"/>
-        <v>210</v>
-      </c>
-      <c r="K32" s="2">
-        <f t="shared" si="3"/>
         <v>1553.1000000000001</v>
       </c>
       <c r="L32" s="1"/>
@@ -3396,22 +3396,22 @@
     </row>
     <row r="33" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C33" s="2">
+        <f t="shared" si="4"/>
+        <v>55</v>
+      </c>
+      <c r="D33" s="2">
         <f t="shared" si="5"/>
-        <v>55</v>
-      </c>
-      <c r="D33" s="2">
+        <v>24.200000000000003</v>
+      </c>
+      <c r="E33" s="2">
         <f t="shared" si="0"/>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="E33" s="2">
-        <f t="shared" si="1"/>
         <v>1331.0000000000002</v>
       </c>
       <c r="F33" s="4">
@@ -3431,11 +3431,11 @@
         <v>10</v>
       </c>
       <c r="J33" s="2">
+        <f t="shared" si="1"/>
+        <v>220</v>
+      </c>
+      <c r="K33" s="2">
         <f t="shared" si="2"/>
-        <v>220</v>
-      </c>
-      <c r="K33" s="2">
-        <f t="shared" si="3"/>
         <v>1551.0000000000002</v>
       </c>
       <c r="L33" s="1"/>
@@ -3486,22 +3486,22 @@
     </row>
     <row r="34" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C34" s="2">
+        <f t="shared" si="4"/>
+        <v>54.5</v>
+      </c>
+      <c r="D34" s="2">
         <f t="shared" si="5"/>
-        <v>54.5</v>
-      </c>
-      <c r="D34" s="2">
+        <v>24.200000000000003</v>
+      </c>
+      <c r="E34" s="2">
         <f t="shared" si="0"/>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="E34" s="2">
-        <f t="shared" si="1"/>
         <v>1318.9</v>
       </c>
       <c r="F34" s="4">
@@ -3521,11 +3521,11 @@
         <v>10</v>
       </c>
       <c r="J34" s="2">
+        <f t="shared" si="1"/>
+        <v>230</v>
+      </c>
+      <c r="K34" s="2">
         <f t="shared" si="2"/>
-        <v>230</v>
-      </c>
-      <c r="K34" s="2">
-        <f t="shared" si="3"/>
         <v>1548.9</v>
       </c>
       <c r="L34" s="1"/>
@@ -3576,22 +3576,22 @@
     </row>
     <row r="35" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>33</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C35" s="2">
+        <f t="shared" si="4"/>
+        <v>54</v>
+      </c>
+      <c r="D35" s="2">
         <f t="shared" si="5"/>
-        <v>54</v>
-      </c>
-      <c r="D35" s="2">
-        <f>22*1.1/2</f>
         <v>12.100000000000001</v>
       </c>
       <c r="E35" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>653.40000000000009</v>
       </c>
       <c r="F35" s="4">
@@ -3611,11 +3611,11 @@
         <v>10</v>
       </c>
       <c r="J35" s="2">
+        <f t="shared" si="1"/>
+        <v>240</v>
+      </c>
+      <c r="K35" s="2">
         <f t="shared" si="2"/>
-        <v>240</v>
-      </c>
-      <c r="K35" s="2">
-        <f t="shared" si="3"/>
         <v>893.40000000000009</v>
       </c>
       <c r="L35" s="1"/>
@@ -3666,22 +3666,22 @@
     </row>
     <row r="36" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>34</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C36" s="2">
+        <f t="shared" si="4"/>
+        <v>53.5</v>
+      </c>
+      <c r="D36" s="2">
         <f t="shared" si="5"/>
-        <v>53.5</v>
-      </c>
-      <c r="D36" s="2">
-        <f t="shared" ref="D36:D38" si="10">22*1.1/2</f>
         <v>12.100000000000001</v>
       </c>
       <c r="E36" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>647.35</v>
       </c>
       <c r="F36" s="4">
@@ -3701,11 +3701,11 @@
         <v>10</v>
       </c>
       <c r="J36" s="2">
+        <f t="shared" si="1"/>
+        <v>250</v>
+      </c>
+      <c r="K36" s="2">
         <f t="shared" si="2"/>
-        <v>250</v>
-      </c>
-      <c r="K36" s="2">
-        <f t="shared" si="3"/>
         <v>897.35</v>
       </c>
       <c r="L36" s="1"/>
@@ -3756,22 +3756,22 @@
     </row>
     <row r="37" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C37" s="2">
+        <f t="shared" si="4"/>
+        <v>53</v>
+      </c>
+      <c r="D37" s="2">
         <f t="shared" si="5"/>
-        <v>53</v>
-      </c>
-      <c r="D37" s="2">
-        <f t="shared" si="10"/>
         <v>12.100000000000001</v>
       </c>
       <c r="E37" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>641.30000000000007</v>
       </c>
       <c r="F37" s="4">
@@ -3791,11 +3791,11 @@
         <v>10</v>
       </c>
       <c r="J37" s="2">
+        <f t="shared" si="1"/>
+        <v>260</v>
+      </c>
+      <c r="K37" s="2">
         <f t="shared" si="2"/>
-        <v>260</v>
-      </c>
-      <c r="K37" s="2">
-        <f t="shared" si="3"/>
         <v>901.30000000000007</v>
       </c>
       <c r="L37" s="1"/>
@@ -3846,22 +3846,22 @@
     </row>
     <row r="38" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C38" s="2">
+        <f t="shared" si="4"/>
+        <v>52.5</v>
+      </c>
+      <c r="D38" s="2">
         <f t="shared" si="5"/>
-        <v>52.5</v>
-      </c>
-      <c r="D38" s="2">
-        <f t="shared" si="10"/>
         <v>12.100000000000001</v>
       </c>
       <c r="E38" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>635.25000000000011</v>
       </c>
       <c r="F38" s="4">
@@ -3881,11 +3881,11 @@
         <v>10</v>
       </c>
       <c r="J38" s="2">
+        <f t="shared" si="1"/>
+        <v>270</v>
+      </c>
+      <c r="K38" s="2">
         <f t="shared" si="2"/>
-        <v>270</v>
-      </c>
-      <c r="K38" s="2">
-        <f t="shared" si="3"/>
         <v>905.25000000000011</v>
       </c>
       <c r="L38" s="1"/>
@@ -4058,7 +4058,7 @@
     <row r="41" spans="1:56" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C41" s="2">
         <f>AVERAGE(C3:C38)</f>
@@ -4121,7 +4121,7 @@
     <row r="42" spans="1:56" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C42" s="2">
         <f>MAX(H3:H38)</f>
@@ -4184,7 +4184,7 @@
     <row r="43" spans="1:56" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C43" s="2">
         <f>MAX(K3:K38)</f>

</xml_diff>

<commit_message>
Sending 1_22_xlsx - try 8 ¯\_(ツ)_/¯
</commit_message>
<xml_diff>
--- a/LR3/table_1_22.xlsx
+++ b/LR3/table_1_22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B34FBC89-9055-48C9-A604-E881A5076513}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E57F085-ADBB-4E74-9DBD-B3D0C0B7D33B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="18912" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,9 +72,6 @@
     <t>Мифтахов</t>
   </si>
   <si>
-    <t>Ма́тижева</t>
-  </si>
-  <si>
     <t>Лучин</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
     <t>Гагаркин</t>
   </si>
   <si>
-    <t>Башкиро́ва</t>
-  </si>
-  <si>
     <t>Байрамшин</t>
   </si>
   <si>
@@ -184,6 +178,12 @@
   </si>
   <si>
     <t>Срок оплаты, день</t>
+  </si>
+  <si>
+    <t>Башкирова</t>
+  </si>
+  <si>
+    <t>Матижева</t>
   </si>
 </sst>
 </file>
@@ -543,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -582,7 +582,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
@@ -591,25 +591,25 @@
         <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -617,7 +617,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1">
         <v>70</v>
@@ -658,7 +658,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1">
         <f>C3-0.5</f>
@@ -703,7 +703,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" ref="C5:C38" si="5">C4-0.5</f>
@@ -748,7 +748,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="5"/>
@@ -793,7 +793,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" si="5"/>
@@ -838,7 +838,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" si="5"/>
@@ -883,7 +883,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" si="5"/>
@@ -928,7 +928,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" si="5"/>
@@ -973,7 +973,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1">
         <f t="shared" si="5"/>
@@ -1018,7 +1018,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" si="5"/>
@@ -1513,7 +1513,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C23" s="1">
         <f t="shared" si="5"/>
@@ -1558,7 +1558,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C24" s="1">
         <f t="shared" si="5"/>
@@ -1603,7 +1603,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C25" s="1">
         <f t="shared" si="5"/>
@@ -1648,7 +1648,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C26" s="1">
         <f t="shared" si="5"/>
@@ -1693,7 +1693,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C27" s="1">
         <f t="shared" si="5"/>
@@ -1738,7 +1738,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C28" s="1">
         <f t="shared" si="5"/>
@@ -1783,7 +1783,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C29" s="1">
         <f t="shared" si="5"/>
@@ -1828,7 +1828,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C30" s="1">
         <f t="shared" si="5"/>
@@ -1873,7 +1873,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C31" s="1">
         <f t="shared" si="5"/>
@@ -1918,7 +1918,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C32" s="1">
         <f t="shared" si="5"/>
@@ -1963,7 +1963,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C33" s="1">
         <f t="shared" si="5"/>
@@ -2008,7 +2008,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C34" s="1">
         <f t="shared" si="5"/>
@@ -2053,7 +2053,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C35" s="1">
         <f t="shared" si="5"/>
@@ -2098,7 +2098,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C36" s="1">
         <f t="shared" si="5"/>
@@ -2143,7 +2143,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C37" s="1">
         <f t="shared" si="5"/>
@@ -2188,7 +2188,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C38" s="1">
         <f t="shared" si="5"/>
@@ -2242,7 +2242,7 @@
     <row r="40" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C40" s="6">
         <f>SUM(K3:K38)</f>
@@ -2260,7 +2260,7 @@
     <row r="41" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C41" s="7">
         <f>AVERAGE(C3:C38)</f>
@@ -2278,7 +2278,7 @@
     <row r="42" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C42" s="1">
         <f>MAX(H3:H38)</f>
@@ -2296,7 +2296,7 @@
     <row r="43" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C43" s="6">
         <f>MAX(K3:K38)</f>

</xml_diff>

<commit_message>
Sending 1_22_xlsx - try 9 ¯\_(ツ)_/¯
</commit_message>
<xml_diff>
--- a/LR3/table_1_22.xlsx
+++ b/LR3/table_1_22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E57F085-ADBB-4E74-9DBD-B3D0C0B7D33B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{68D97691-CEFA-4514-A203-FEA8DE1C533F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="18912" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -543,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -564,7 +564,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -714,7 +714,7 @@
         <v>24.200000000000003</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" si="0"/>
+        <f>D5*C5</f>
         <v>1669.8000000000002</v>
       </c>
       <c r="F5" s="10">

</xml_diff>

<commit_message>
Sending 1_22_xlsx - try 10 ¯\_(ツ)_/¯
</commit_message>
<xml_diff>
--- a/LR3/table_1_22.xlsx
+++ b/LR3/table_1_22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{68D97691-CEFA-4514-A203-FEA8DE1C533F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E48C625-C35B-49A7-AD07-0E2A2E5BA731}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -174,16 +174,16 @@
     <t>Максимальная сумма, руб.</t>
   </si>
   <si>
-    <t>Дата оплаты, день</t>
-  </si>
-  <si>
-    <t>Срок оплаты, день</t>
-  </si>
-  <si>
     <t>Башкирова</t>
   </si>
   <si>
     <t>Матижева</t>
+  </si>
+  <si>
+    <t>Срок оплаты</t>
+  </si>
+  <si>
+    <t>Дата оплаты</t>
   </si>
 </sst>
 </file>
@@ -544,7 +544,7 @@
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -594,10 +594,10 @@
         <v>37</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>38</v>
@@ -703,7 +703,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" ref="C5:C38" si="5">C4-0.5</f>
@@ -1018,7 +1018,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" si="5"/>

</xml_diff>

<commit_message>
Sending 1_22_xlsx - try 11 ¯\_(ツ)_/¯
</commit_message>
<xml_diff>
--- a/LR3/table_1_22.xlsx
+++ b/LR3/table_1_22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E48C625-C35B-49A7-AD07-0E2A2E5BA731}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B8FE963-73CA-4B38-81EE-979C1E58DA70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2880" yWindow="2712" windowWidth="18912" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -190,10 +190,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
-  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -243,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -258,8 +254,6 @@
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -543,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -623,17 +617,17 @@
         <v>70</v>
       </c>
       <c r="D3" s="1">
-        <f>22*1.1</f>
+        <f>$A$1*1.1</f>
         <v>24.200000000000003</v>
       </c>
       <c r="E3" s="1">
-        <f>D3*C3</f>
+        <f>C3*D3</f>
         <v>1694.0000000000002</v>
       </c>
-      <c r="F3" s="10">
-        <v>44813</v>
-      </c>
-      <c r="G3" s="10">
+      <c r="F3" s="8">
+        <v>44813</v>
+      </c>
+      <c r="G3" s="8">
         <v>44805</v>
       </c>
       <c r="H3" s="1">
@@ -644,11 +638,11 @@
         <v>10</v>
       </c>
       <c r="J3" s="1">
-        <f>I3*H3</f>
+        <f>H3*I3</f>
         <v>0</v>
       </c>
       <c r="K3" s="6">
-        <f>SUM(E3,J3)</f>
+        <f>E3+J3</f>
         <v>1694.0000000000002</v>
       </c>
     </row>
@@ -665,113 +659,113 @@
         <v>69.5</v>
       </c>
       <c r="D4" s="1">
-        <f>IF((A4 / 4 &lt;= 8),$D$3, $D$3/2)</f>
+        <f t="shared" ref="D4:D34" si="0">$A$1*1.1</f>
         <v>24.200000000000003</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" ref="E4:E38" si="0">D4*C4</f>
+        <f t="shared" ref="E4:E38" si="1">C4*D4</f>
         <v>1681.9</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="8">
         <f>$F$3</f>
         <v>44813</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="8">
         <f>G3+1</f>
         <v>44806</v>
       </c>
       <c r="H4" s="1">
-        <f t="shared" ref="H4:H38" si="1">IF(G4&lt;=F4, 0, G4-F4)</f>
+        <f t="shared" ref="H4:H38" si="2">IF(G4&lt;=F4, 0, G4-F4)</f>
         <v>0</v>
       </c>
       <c r="I4" s="1">
-        <f>$I$3</f>
+        <f>I3</f>
         <v>10</v>
       </c>
       <c r="J4" s="1">
-        <f t="shared" ref="J4:J11" si="2">I4*H4</f>
+        <f t="shared" ref="J4:J38" si="3">H4*I4</f>
         <v>0</v>
       </c>
-      <c r="K4" s="7">
-        <f t="shared" ref="K4:K38" si="3">SUM(E4,J4)</f>
+      <c r="K4" s="6">
+        <f t="shared" ref="K4:K38" si="4">E4+J4</f>
         <v>1681.9</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <f t="shared" ref="A5:A38" si="4">A4+1</f>
+        <f t="shared" ref="A5:A38" si="5">A4+1</f>
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>47</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" ref="C5:C38" si="5">C4-0.5</f>
+        <f t="shared" ref="C5:C38" si="6">C4-0.5</f>
         <v>69</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" ref="D5:D38" si="6">IF((A5 / 4 &lt;= 8),$D$3, $D$3/2)</f>
+        <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
       <c r="E5" s="1">
-        <f>D5*C5</f>
+        <f t="shared" si="1"/>
         <v>1669.8000000000002</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="8">
         <f t="shared" ref="F5:F37" si="7">$F$3</f>
         <v>44813</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="8">
         <f t="shared" ref="G5:G38" si="8">G4+1</f>
         <v>44807</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" ref="I5:I37" si="9">$I$3</f>
+        <f t="shared" ref="I5:I38" si="9">I4</f>
         <v>10</v>
       </c>
       <c r="J5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K5" s="8">
-        <f t="shared" si="3"/>
+      <c r="K5" s="6">
+        <f t="shared" si="4"/>
         <v>1669.8000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>68.5</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1657.7000000000003</v>
       </c>
-      <c r="F6" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G6" s="10">
+      <c r="F6" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G6" s="8">
         <f t="shared" si="8"/>
         <v>44808</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I6" s="1">
@@ -779,44 +773,44 @@
         <v>10</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K6" s="7">
-        <f t="shared" si="3"/>
+      <c r="K6" s="6">
+        <f t="shared" si="4"/>
         <v>1657.7000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>68</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1645.6000000000001</v>
       </c>
-      <c r="F7" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G7" s="10">
+      <c r="F7" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G7" s="8">
         <f t="shared" si="8"/>
         <v>44809</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I7" s="1">
@@ -824,44 +818,44 @@
         <v>10</v>
       </c>
       <c r="J7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K7" s="8">
-        <f t="shared" si="3"/>
+      <c r="K7" s="6">
+        <f t="shared" si="4"/>
         <v>1645.6000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>67.5</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1633.5000000000002</v>
       </c>
-      <c r="F8" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G8" s="10">
+      <c r="F8" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G8" s="8">
         <f t="shared" si="8"/>
         <v>44810</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I8" s="1">
@@ -869,44 +863,44 @@
         <v>10</v>
       </c>
       <c r="J8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K8" s="7">
-        <f t="shared" si="3"/>
+      <c r="K8" s="6">
+        <f t="shared" si="4"/>
         <v>1633.5000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>67</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1621.4</v>
       </c>
-      <c r="F9" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G9" s="10">
+      <c r="F9" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G9" s="8">
         <f t="shared" si="8"/>
         <v>44811</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I9" s="1">
@@ -914,44 +908,44 @@
         <v>10</v>
       </c>
       <c r="J9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K9" s="8">
-        <f t="shared" si="3"/>
+      <c r="K9" s="6">
+        <f t="shared" si="4"/>
         <v>1621.4</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>66.5</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1609.3000000000002</v>
       </c>
-      <c r="F10" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G10" s="10">
+      <c r="F10" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G10" s="8">
         <f t="shared" si="8"/>
         <v>44812</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I10" s="1">
@@ -959,44 +953,44 @@
         <v>10</v>
       </c>
       <c r="J10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K10" s="7">
-        <f t="shared" si="3"/>
+      <c r="K10" s="6">
+        <f t="shared" si="4"/>
         <v>1609.3000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>66</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1597.2000000000003</v>
       </c>
-      <c r="F11" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G11" s="10">
+      <c r="F11" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G11" s="8">
         <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I11" s="1">
@@ -1004,44 +998,44 @@
         <v>10</v>
       </c>
       <c r="J11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K11" s="8">
-        <f t="shared" si="3"/>
+      <c r="K11" s="6">
+        <f t="shared" si="4"/>
         <v>1597.2000000000003</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C12" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>65.5</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1585.1000000000001</v>
       </c>
-      <c r="F12" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G12" s="10">
+      <c r="F12" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G12" s="8">
         <f t="shared" si="8"/>
         <v>44814</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I12" s="1">
@@ -1049,44 +1043,44 @@
         <v>10</v>
       </c>
       <c r="J12" s="1">
-        <f>I12*H12</f>
-        <v>10</v>
-      </c>
-      <c r="K12" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="K12" s="6">
+        <f t="shared" si="4"/>
         <v>1595.1000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>65</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1573.0000000000002</v>
       </c>
-      <c r="F13" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G13" s="10">
+      <c r="F13" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G13" s="8">
         <f t="shared" si="8"/>
         <v>44815</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I13" s="1">
@@ -1094,44 +1088,44 @@
         <v>10</v>
       </c>
       <c r="J13" s="1">
-        <f>I13*H13</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="K13" s="8">
-        <f t="shared" si="3"/>
+      <c r="K13" s="6">
+        <f t="shared" si="4"/>
         <v>1593.0000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>64.5</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1560.9</v>
       </c>
-      <c r="F14" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G14" s="10">
+      <c r="F14" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G14" s="8">
         <f t="shared" si="8"/>
         <v>44816</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I14" s="1">
@@ -1139,44 +1133,44 @@
         <v>10</v>
       </c>
       <c r="J14" s="1">
-        <f t="shared" ref="J14:J38" si="10">I14*H14</f>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="K14" s="7">
-        <f t="shared" si="3"/>
+      <c r="K14" s="6">
+        <f t="shared" si="4"/>
         <v>1590.9</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>64</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1548.8000000000002</v>
       </c>
-      <c r="F15" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G15" s="10">
+      <c r="F15" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G15" s="8">
         <f t="shared" si="8"/>
         <v>44817</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I15" s="1">
@@ -1184,44 +1178,44 @@
         <v>10</v>
       </c>
       <c r="J15" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="K15" s="8">
-        <f t="shared" si="3"/>
+      <c r="K15" s="6">
+        <f t="shared" si="4"/>
         <v>1588.8000000000002</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>63.5</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
       <c r="E16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1536.7000000000003</v>
       </c>
-      <c r="F16" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G16" s="10">
+      <c r="F16" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G16" s="8">
         <f t="shared" si="8"/>
         <v>44818</v>
       </c>
       <c r="H16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I16" s="1">
@@ -1229,44 +1223,44 @@
         <v>10</v>
       </c>
       <c r="J16" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="K16" s="7">
-        <f t="shared" si="3"/>
+      <c r="K16" s="6">
+        <f t="shared" si="4"/>
         <v>1586.7000000000003</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>63</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
       <c r="E17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1524.6000000000001</v>
       </c>
-      <c r="F17" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G17" s="10">
+      <c r="F17" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G17" s="8">
         <f t="shared" si="8"/>
         <v>44819</v>
       </c>
       <c r="H17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="I17" s="1">
@@ -1274,44 +1268,44 @@
         <v>10</v>
       </c>
       <c r="J17" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
-      <c r="K17" s="8">
-        <f t="shared" si="3"/>
+      <c r="K17" s="6">
+        <f t="shared" si="4"/>
         <v>1584.6000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>62.5</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1512.5000000000002</v>
       </c>
-      <c r="F18" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G18" s="10">
+      <c r="F18" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G18" s="8">
         <f t="shared" si="8"/>
         <v>44820</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="I18" s="1">
@@ -1319,44 +1313,44 @@
         <v>10</v>
       </c>
       <c r="J18" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
-      <c r="K18" s="7">
-        <f t="shared" si="3"/>
+      <c r="K18" s="6">
+        <f t="shared" si="4"/>
         <v>1582.5000000000002</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>62</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1500.4</v>
       </c>
-      <c r="F19" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G19" s="10">
+      <c r="F19" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G19" s="8">
         <f t="shared" si="8"/>
         <v>44821</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="I19" s="1">
@@ -1364,44 +1358,44 @@
         <v>10</v>
       </c>
       <c r="J19" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>80</v>
       </c>
-      <c r="K19" s="8">
-        <f t="shared" si="3"/>
+      <c r="K19" s="6">
+        <f t="shared" si="4"/>
         <v>1580.4</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>61.5</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
       <c r="E20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1488.3000000000002</v>
       </c>
-      <c r="F20" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G20" s="10">
+      <c r="F20" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G20" s="8">
         <f t="shared" si="8"/>
         <v>44822</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="I20" s="1">
@@ -1409,44 +1403,44 @@
         <v>10</v>
       </c>
       <c r="J20" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="K20" s="7">
-        <f t="shared" si="3"/>
+      <c r="K20" s="6">
+        <f t="shared" si="4"/>
         <v>1578.3000000000002</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C21" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>61</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
       <c r="E21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1476.2000000000003</v>
       </c>
-      <c r="F21" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G21" s="10">
+      <c r="F21" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G21" s="8">
         <f t="shared" si="8"/>
         <v>44823</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="I21" s="1">
@@ -1454,44 +1448,44 @@
         <v>10</v>
       </c>
       <c r="J21" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="K21" s="8">
-        <f t="shared" si="3"/>
+      <c r="K21" s="6">
+        <f t="shared" si="4"/>
         <v>1576.2000000000003</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>60.5</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
       <c r="E22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1464.1000000000001</v>
       </c>
-      <c r="F22" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G22" s="10">
+      <c r="F22" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G22" s="8">
         <f t="shared" si="8"/>
         <v>44824</v>
       </c>
       <c r="H22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="I22" s="1">
@@ -1499,44 +1493,44 @@
         <v>10</v>
       </c>
       <c r="J22" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>110</v>
       </c>
-      <c r="K22" s="7">
-        <f t="shared" si="3"/>
+      <c r="K22" s="6">
+        <f t="shared" si="4"/>
         <v>1574.1000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>60</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
       <c r="E23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1452.0000000000002</v>
       </c>
-      <c r="F23" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G23" s="10">
+      <c r="F23" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G23" s="8">
         <f t="shared" si="8"/>
         <v>44825</v>
       </c>
       <c r="H23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="I23" s="1">
@@ -1544,44 +1538,44 @@
         <v>10</v>
       </c>
       <c r="J23" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>120</v>
       </c>
       <c r="K23" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1572.0000000000002</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C24" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>59.5</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
       <c r="E24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1439.9</v>
       </c>
-      <c r="F24" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G24" s="10">
+      <c r="F24" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G24" s="8">
         <f t="shared" si="8"/>
         <v>44826</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="I24" s="1">
@@ -1589,44 +1583,44 @@
         <v>10</v>
       </c>
       <c r="J24" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>130</v>
       </c>
-      <c r="K24" s="7">
-        <f t="shared" si="3"/>
+      <c r="K24" s="6">
+        <f t="shared" si="4"/>
         <v>1569.9</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>59</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
       <c r="E25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1427.8000000000002</v>
       </c>
-      <c r="F25" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G25" s="10">
+      <c r="F25" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G25" s="8">
         <f t="shared" si="8"/>
         <v>44827</v>
       </c>
       <c r="H25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="I25" s="1">
@@ -1634,44 +1628,44 @@
         <v>10</v>
       </c>
       <c r="J25" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>140</v>
       </c>
-      <c r="K25" s="8">
-        <f t="shared" si="3"/>
+      <c r="K25" s="6">
+        <f t="shared" si="4"/>
         <v>1567.8000000000002</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C26" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>58.5</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
       <c r="E26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1415.7000000000003</v>
       </c>
-      <c r="F26" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G26" s="10">
+      <c r="F26" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G26" s="8">
         <f t="shared" si="8"/>
         <v>44828</v>
       </c>
       <c r="H26" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="I26" s="1">
@@ -1679,44 +1673,44 @@
         <v>10</v>
       </c>
       <c r="J26" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>150</v>
       </c>
-      <c r="K26" s="7">
-        <f t="shared" si="3"/>
+      <c r="K26" s="6">
+        <f t="shared" si="4"/>
         <v>1565.7000000000003</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C27" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>58</v>
       </c>
       <c r="D27" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
       <c r="E27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1403.6000000000001</v>
       </c>
-      <c r="F27" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G27" s="10">
+      <c r="F27" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G27" s="8">
         <f t="shared" si="8"/>
         <v>44829</v>
       </c>
       <c r="H27" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="I27" s="1">
@@ -1724,44 +1718,44 @@
         <v>10</v>
       </c>
       <c r="J27" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>160</v>
       </c>
-      <c r="K27" s="8">
-        <f t="shared" si="3"/>
+      <c r="K27" s="6">
+        <f t="shared" si="4"/>
         <v>1563.6000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C28" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>57.5</v>
       </c>
       <c r="D28" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
       <c r="E28" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1391.5000000000002</v>
       </c>
-      <c r="F28" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G28" s="10">
+      <c r="F28" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G28" s="8">
         <f t="shared" si="8"/>
         <v>44830</v>
       </c>
       <c r="H28" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="I28" s="1">
@@ -1769,44 +1763,44 @@
         <v>10</v>
       </c>
       <c r="J28" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>170</v>
       </c>
-      <c r="K28" s="7">
-        <f t="shared" si="3"/>
+      <c r="K28" s="6">
+        <f t="shared" si="4"/>
         <v>1561.5000000000002</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C29" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>57</v>
       </c>
       <c r="D29" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
       <c r="E29" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1379.4</v>
       </c>
-      <c r="F29" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G29" s="10">
+      <c r="F29" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G29" s="8">
         <f t="shared" si="8"/>
         <v>44831</v>
       </c>
       <c r="H29" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="I29" s="1">
@@ -1814,44 +1808,44 @@
         <v>10</v>
       </c>
       <c r="J29" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>180</v>
       </c>
-      <c r="K29" s="8">
-        <f t="shared" si="3"/>
+      <c r="K29" s="6">
+        <f t="shared" si="4"/>
         <v>1559.4</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C30" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>56.5</v>
       </c>
       <c r="D30" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
       <c r="E30" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1367.3000000000002</v>
       </c>
-      <c r="F30" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G30" s="10">
+      <c r="F30" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G30" s="8">
         <f t="shared" si="8"/>
         <v>44832</v>
       </c>
       <c r="H30" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="I30" s="1">
@@ -1859,44 +1853,44 @@
         <v>10</v>
       </c>
       <c r="J30" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>190</v>
       </c>
-      <c r="K30" s="7">
-        <f t="shared" si="3"/>
+      <c r="K30" s="6">
+        <f t="shared" si="4"/>
         <v>1557.3000000000002</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C31" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>56</v>
       </c>
       <c r="D31" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
       <c r="E31" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1355.2000000000003</v>
       </c>
-      <c r="F31" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G31" s="10">
+      <c r="F31" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G31" s="8">
         <f t="shared" si="8"/>
         <v>44833</v>
       </c>
       <c r="H31" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="I31" s="1">
@@ -1904,44 +1898,44 @@
         <v>10</v>
       </c>
       <c r="J31" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>200</v>
       </c>
-      <c r="K31" s="8">
-        <f t="shared" si="3"/>
+      <c r="K31" s="6">
+        <f t="shared" si="4"/>
         <v>1555.2000000000003</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C32" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>55.5</v>
       </c>
       <c r="D32" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
       <c r="E32" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1343.1000000000001</v>
       </c>
-      <c r="F32" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G32" s="10">
+      <c r="F32" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G32" s="8">
         <f t="shared" si="8"/>
         <v>44834</v>
       </c>
       <c r="H32" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="I32" s="1">
@@ -1949,44 +1943,44 @@
         <v>10</v>
       </c>
       <c r="J32" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>210</v>
       </c>
-      <c r="K32" s="7">
-        <f t="shared" si="3"/>
+      <c r="K32" s="6">
+        <f t="shared" si="4"/>
         <v>1553.1000000000001</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C33" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="D33" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
       <c r="E33" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1331.0000000000002</v>
       </c>
-      <c r="F33" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G33" s="10">
+      <c r="F33" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G33" s="8">
         <f t="shared" si="8"/>
         <v>44835</v>
       </c>
       <c r="H33" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="I33" s="1">
@@ -1994,44 +1988,44 @@
         <v>10</v>
       </c>
       <c r="J33" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>220</v>
       </c>
-      <c r="K33" s="8">
-        <f t="shared" si="3"/>
+      <c r="K33" s="6">
+        <f t="shared" si="4"/>
         <v>1551.0000000000002</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C34" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>54.5</v>
       </c>
       <c r="D34" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
       <c r="E34" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1318.9</v>
       </c>
-      <c r="F34" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G34" s="10">
+      <c r="F34" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G34" s="8">
         <f t="shared" si="8"/>
         <v>44836</v>
       </c>
       <c r="H34" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="I34" s="1">
@@ -2039,44 +2033,44 @@
         <v>10</v>
       </c>
       <c r="J34" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>230</v>
       </c>
-      <c r="K34" s="7">
-        <f t="shared" si="3"/>
+      <c r="K34" s="6">
+        <f t="shared" si="4"/>
         <v>1548.9</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C35" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>54</v>
       </c>
       <c r="D35" s="1">
-        <f t="shared" si="6"/>
+        <f>$A$1*1.1/2</f>
         <v>12.100000000000001</v>
       </c>
       <c r="E35" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>653.40000000000009</v>
       </c>
-      <c r="F35" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G35" s="10">
+      <c r="F35" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G35" s="8">
         <f t="shared" si="8"/>
         <v>44837</v>
       </c>
       <c r="H35" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="I35" s="1">
@@ -2084,44 +2078,44 @@
         <v>10</v>
       </c>
       <c r="J35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>240</v>
       </c>
-      <c r="K35" s="8">
-        <f t="shared" si="3"/>
+      <c r="K35" s="6">
+        <f t="shared" si="4"/>
         <v>893.40000000000009</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C36" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>53.5</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="D36:D38" si="10">$A$1*1.1/2</f>
         <v>12.100000000000001</v>
       </c>
       <c r="E36" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>647.35</v>
       </c>
-      <c r="F36" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G36" s="10">
+      <c r="F36" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G36" s="8">
         <f t="shared" si="8"/>
         <v>44838</v>
       </c>
       <c r="H36" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="I36" s="1">
@@ -2129,44 +2123,44 @@
         <v>10</v>
       </c>
       <c r="J36" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>250</v>
       </c>
-      <c r="K36" s="9">
-        <f t="shared" si="3"/>
+      <c r="K36" s="6">
+        <f t="shared" si="4"/>
         <v>897.35</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C37" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>53</v>
       </c>
       <c r="D37" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>12.100000000000001</v>
       </c>
       <c r="E37" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>641.30000000000007</v>
       </c>
-      <c r="F37" s="10">
-        <f t="shared" si="7"/>
-        <v>44813</v>
-      </c>
-      <c r="G37" s="10">
+      <c r="F37" s="8">
+        <f t="shared" si="7"/>
+        <v>44813</v>
+      </c>
+      <c r="G37" s="8">
         <f t="shared" si="8"/>
         <v>44839</v>
       </c>
       <c r="H37" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="I37" s="1">
@@ -2174,55 +2168,56 @@
         <v>10</v>
       </c>
       <c r="J37" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>260</v>
       </c>
-      <c r="K37" s="7">
-        <f t="shared" si="3"/>
+      <c r="K37" s="6">
+        <f t="shared" si="4"/>
         <v>901.30000000000007</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C38" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>52.5</v>
       </c>
       <c r="D38" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>12.100000000000001</v>
       </c>
       <c r="E38" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>635.25000000000011</v>
       </c>
-      <c r="F38" s="10">
+      <c r="F38" s="8">
         <f>$F$3</f>
         <v>44813</v>
       </c>
-      <c r="G38" s="10">
+      <c r="G38" s="8">
         <f t="shared" si="8"/>
         <v>44840</v>
       </c>
       <c r="H38" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="I38" s="1">
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J38" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>270</v>
       </c>
-      <c r="K38" s="9">
-        <f t="shared" si="3"/>
+      <c r="K38" s="6">
+        <f t="shared" si="4"/>
         <v>905.25000000000011</v>
       </c>
     </row>
@@ -2233,7 +2228,7 @@
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
-      <c r="G39" s="10"/>
+      <c r="G39" s="8"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
@@ -2245,8 +2240,8 @@
         <v>45</v>
       </c>
       <c r="C40" s="6">
-        <f>SUM(K3:K38)</f>
-        <v>54563.700000000004</v>
+        <f>FLOOR(SUM(K3:K38),1)</f>
+        <v>54563</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>

</xml_diff>

<commit_message>
Sending 1_22_xlsx - try 12 ¯\_(ツ)_/¯
</commit_message>
<xml_diff>
--- a/LR3/table_1_22.xlsx
+++ b/LR3/table_1_22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B8FE963-73CA-4B38-81EE-979C1E58DA70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A94703F-3449-4150-A1F5-0253B2367136}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="2712" windowWidth="18912" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5856" yWindow="1980" windowWidth="18912" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -537,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -631,7 +631,7 @@
         <v>44805</v>
       </c>
       <c r="H3" s="1">
-        <f>IF(G3&lt;=F3, 0, G3-F3)</f>
+        <f>IF(G3&lt;=F3,0,G3-F3)</f>
         <v>0</v>
       </c>
       <c r="I3" s="1">
@@ -675,7 +675,7 @@
         <v>44806</v>
       </c>
       <c r="H4" s="1">
-        <f t="shared" ref="H4:H38" si="2">IF(G4&lt;=F4, 0, G4-F4)</f>
+        <f t="shared" ref="H4:H38" si="2">IF(G4&lt;=F4,0,G4-F4)</f>
         <v>0</v>
       </c>
       <c r="I4" s="1">

</xml_diff>